<commit_message>
update for db api: show the dataset_type field in the output
</commit_message>
<xml_diff>
--- a/sampledata/Screen20020_HMSL10008_kinomescan.xlsx
+++ b/sampledata/Screen20020_HMSL10008_kinomescan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="58">
   <si>
     <t>Field</t>
   </si>
@@ -76,7 +76,7 @@
     <t>Summary</t>
   </si>
   <si>
-    <t>The KINOMEscan assay platform is based on a competition binding assay that is run for a compound of interest against each of a panel of 317 to 456 kinases. The assay has three components: a kinase-tagged phage, a test compound, and an immobilized ligand that the compound competes with to displace the kinase. The amount of kinase bound to the immobilized ligand is determined using quantitative PCR of the DNA tag.  Results for each kinase are reported as "Percent of control", where the control is DMSO and where a 100% result means no inhibition of kinase binding to the ligand in the presence of the compound, and where low percent results mean strong inhibition. The KINOMEscan data are presented graphically on TREEspot Kinase Dendrograms (http://www.kinomescan.com/Tools---Resources/Study-Reports---Data-Analysis).  For this study, HMS LINCS investigators have graphed results for kinases classified as 35 "percent of control" (in the presence of the compound, the kinase is 35% as active for binding ligand in the presence of DMSO), 5 "percent of control" and 1 "percent of control". </t>
+    <t>The KINOMEscan assay platform is based on a competition binding assay that is run for a compound of interest against each of a panel of 317 to 456 kinases. The assay has three components: a kinase-tagged phage, a test compound, and an immobilized ligand that the compound competes with to displace the kinase. The amount of kinase bound to the immobilized ligand is determined using quantitative PCR of the DNA tag.  Results for each kinase are reported as "Percent of control", where the control is DMSO and where a 100% result means no inhibition of kinase binding to the ligand in the presence of the compound, and where low percent results mean strong inhibition. The KINOMEscan data are presented graphically on TREEspot Kinase Dendrograms (http://www.kinomescan.com/Tools---Resources/Study-Reports---Data-Analysis).  For this study, HMS LINCS investigators have graphed results for kinases classified as 35 "percent of control" (in the presence of the compound, the kinase is 35% as active for binding ligand in the presence of DMSO), 5 "percent of control" and 1 "percent of control".</t>
   </si>
   <si>
     <t>Protocol</t>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Is Restricted</t>
+  </si>
+  <si>
+    <t>Dataset Type</t>
+  </si>
+  <si>
+    <t>KINOMEscan</t>
   </si>
   <si>
     <t>"Data" Worksheet Column</t>
@@ -302,22 +308,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B17" activeCellId="0" pane="topLeft" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.6117647058824"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="162.364705882353"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="11.6117647058824"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="162.364705882353"/>
-    <col collapsed="false" hidden="false" max="513" min="259" style="1" width="11.6117647058824"/>
-    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="162.364705882353"/>
-    <col collapsed="false" hidden="false" max="769" min="515" style="1" width="11.6117647058824"/>
-    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="162.364705882353"/>
-    <col collapsed="false" hidden="false" max="1025" min="771" style="1" width="11.6117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="163.16862745098"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="163.16862745098"/>
+    <col collapsed="false" hidden="false" max="513" min="259" style="1" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="163.16862745098"/>
+    <col collapsed="false" hidden="false" max="769" min="515" style="1" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="163.16862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="771" style="1" width="11.6666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -443,6 +449,14 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -463,50 +477,50 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B8" activeCellId="0" pane="topLeft" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.721568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
@@ -514,45 +528,45 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -578,45 +592,45 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5450980392157"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.35294117647059"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.68627450980392"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.12549019607843"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.03529411764706"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5058823529412"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.70588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.643137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.38039215686275"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.71372549019608"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.15294117647059"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.07450980392157"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.556862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.74117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>200001</v>
@@ -627,7 +641,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>200004</v>
@@ -638,7 +652,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>200006</v>
@@ -649,7 +663,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>200007</v>
@@ -660,7 +674,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>200009</v>
@@ -671,7 +685,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>200010</v>
@@ -682,7 +696,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>200012</v>
@@ -693,7 +707,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>200013</v>
@@ -704,7 +718,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>200015</v>
@@ -715,7 +729,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>200017</v>
@@ -726,7 +740,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>200018</v>
@@ -737,7 +751,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>200020</v>
@@ -748,7 +762,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>200021</v>
@@ -759,7 +773,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>200023</v>
@@ -770,7 +784,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>200024</v>
@@ -781,7 +795,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>200025</v>
@@ -792,7 +806,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>200026</v>
@@ -803,7 +817,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>200027</v>
@@ -814,7 +828,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>200028</v>
@@ -825,7 +839,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>200029</v>
@@ -836,7 +850,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>200030</v>
@@ -847,7 +861,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>200031</v>
@@ -858,7 +872,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>200032</v>
@@ -869,7 +883,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>200033</v>
@@ -880,7 +894,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>200034</v>
@@ -891,7 +905,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>200035</v>
@@ -902,7 +916,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>200036</v>
@@ -913,7 +927,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>200037</v>
@@ -924,7 +938,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>200038</v>
@@ -935,7 +949,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>200039</v>
@@ -946,7 +960,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>200040</v>
@@ -957,7 +971,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>200041</v>
@@ -968,7 +982,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>200042</v>
@@ -979,7 +993,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>200043</v>
@@ -990,7 +1004,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>200044</v>
@@ -1001,7 +1015,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>200045</v>
@@ -1012,7 +1026,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>200046</v>
@@ -1023,7 +1037,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>200047</v>
@@ -1034,7 +1048,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>200048</v>
@@ -1045,7 +1059,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>200049</v>
@@ -1056,7 +1070,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>200050</v>
@@ -1067,7 +1081,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>200051</v>
@@ -1078,7 +1092,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>200052</v>
@@ -1089,7 +1103,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>200053</v>
@@ -1100,7 +1114,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>200054</v>
@@ -1111,7 +1125,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>200055</v>
@@ -1122,7 +1136,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>200056</v>
@@ -1133,7 +1147,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>200057</v>
@@ -1144,7 +1158,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="A50" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>200058</v>
@@ -1155,7 +1169,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="A51" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>200059</v>
@@ -1166,7 +1180,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="A52" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>200060</v>
@@ -1177,7 +1191,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>200061</v>
@@ -1188,7 +1202,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>200062</v>
@@ -1199,7 +1213,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>200063</v>
@@ -1210,7 +1224,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>200064</v>
@@ -1221,7 +1235,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="A57" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>200065</v>
@@ -1232,7 +1246,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
       <c r="A58" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>200066</v>
@@ -1243,7 +1257,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="A59" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>200067</v>
@@ -1254,7 +1268,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="A60" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>200068</v>
@@ -1265,7 +1279,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>200069</v>
@@ -1276,7 +1290,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
       <c r="A62" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>200070</v>
@@ -1287,7 +1301,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
       <c r="A63" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>200071</v>
@@ -1298,7 +1312,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
       <c r="A64" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>200072</v>
@@ -1309,7 +1323,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
       <c r="A65" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>200073</v>
@@ -1320,7 +1334,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
       <c r="A66" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>200074</v>
@@ -1331,7 +1345,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
       <c r="A67" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>200075</v>
@@ -1342,7 +1356,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="A68" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>200076</v>
@@ -1353,7 +1367,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
       <c r="A69" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>200077</v>
@@ -1364,7 +1378,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
       <c r="A70" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>200078</v>
@@ -1375,7 +1389,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
       <c r="A71" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>200079</v>
@@ -1386,7 +1400,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
       <c r="A72" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>200080</v>
@@ -1397,7 +1411,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
       <c r="A73" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E73" s="0" t="n">
         <v>200081</v>
@@ -1408,7 +1422,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74">
       <c r="A74" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>200082</v>
@@ -1419,7 +1433,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75">
       <c r="A75" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>200083</v>
@@ -1430,7 +1444,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
       <c r="A76" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>200084</v>
@@ -1441,7 +1455,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="77">
       <c r="A77" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>200085</v>
@@ -1452,7 +1466,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="78">
       <c r="A78" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>200086</v>
@@ -1463,7 +1477,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="79">
       <c r="A79" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>200087</v>
@@ -1474,7 +1488,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="80">
       <c r="A80" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>200088</v>
@@ -1485,7 +1499,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="81">
       <c r="A81" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>200089</v>
@@ -1496,7 +1510,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="82">
       <c r="A82" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>200090</v>
@@ -1507,7 +1521,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
       <c r="A83" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E83" s="0" t="n">
         <v>200091</v>
@@ -1518,7 +1532,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84">
       <c r="A84" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E84" s="0" t="n">
         <v>200092</v>
@@ -1529,7 +1543,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
       <c r="A85" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>200093</v>
@@ -1540,7 +1554,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
       <c r="A86" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>200094</v>
@@ -1551,7 +1565,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
       <c r="A87" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>200095</v>
@@ -1562,7 +1576,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88">
       <c r="A88" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>200096</v>
@@ -1573,7 +1587,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
       <c r="A89" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E89" s="0" t="n">
         <v>200097</v>
@@ -1584,7 +1598,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="90">
       <c r="A90" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>200098</v>
@@ -1595,7 +1609,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="91">
       <c r="A91" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E91" s="0" t="n">
         <v>200099</v>
@@ -1606,7 +1620,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
       <c r="A92" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>200100</v>
@@ -1617,7 +1631,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
       <c r="A93" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E93" s="0" t="n">
         <v>200101</v>
@@ -1628,7 +1642,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
       <c r="A94" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>200102</v>
@@ -1639,7 +1653,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95">
       <c r="A95" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>200103</v>
@@ -1650,7 +1664,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96">
       <c r="A96" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>200104</v>
@@ -1661,7 +1675,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="97">
       <c r="A97" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>200105</v>
@@ -1672,7 +1686,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="98">
       <c r="A98" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E98" s="0" t="n">
         <v>200106</v>
@@ -1683,7 +1697,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="99">
       <c r="A99" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E99" s="0" t="n">
         <v>200107</v>
@@ -1694,7 +1708,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
       <c r="A100" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>200108</v>
@@ -1705,7 +1719,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="101">
       <c r="A101" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E101" s="0" t="n">
         <v>200109</v>
@@ -1716,7 +1730,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="102">
       <c r="A102" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E102" s="0" t="n">
         <v>200110</v>
@@ -1727,7 +1741,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="103">
       <c r="A103" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E103" s="0" t="n">
         <v>200111</v>
@@ -1738,7 +1752,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="104">
       <c r="A104" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E104" s="0" t="n">
         <v>200112</v>
@@ -1749,7 +1763,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="105">
       <c r="A105" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E105" s="0" t="n">
         <v>200113</v>
@@ -1760,7 +1774,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="106">
       <c r="A106" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E106" s="0" t="n">
         <v>200114</v>
@@ -1771,7 +1785,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="107">
       <c r="A107" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E107" s="0" t="n">
         <v>200115</v>
@@ -1782,7 +1796,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="108">
       <c r="A108" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E108" s="0" t="n">
         <v>200116</v>
@@ -1793,7 +1807,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="109">
       <c r="A109" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E109" s="0" t="n">
         <v>200117</v>
@@ -1804,7 +1818,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="110">
       <c r="A110" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E110" s="0" t="n">
         <v>200118</v>
@@ -1815,7 +1829,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="111">
       <c r="A111" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E111" s="0" t="n">
         <v>200119</v>
@@ -1826,7 +1840,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="112">
       <c r="A112" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E112" s="0" t="n">
         <v>200120</v>
@@ -1837,7 +1851,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="113">
       <c r="A113" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E113" s="0" t="n">
         <v>200121</v>
@@ -1848,7 +1862,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="114">
       <c r="A114" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E114" s="0" t="n">
         <v>200122</v>
@@ -1859,7 +1873,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="115">
       <c r="A115" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E115" s="0" t="n">
         <v>200123</v>
@@ -1870,7 +1884,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="116">
       <c r="A116" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E116" s="0" t="n">
         <v>200124</v>
@@ -1881,7 +1895,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="117">
       <c r="A117" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E117" s="0" t="n">
         <v>200125</v>
@@ -1892,7 +1906,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="118">
       <c r="A118" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E118" s="0" t="n">
         <v>200126</v>
@@ -1903,7 +1917,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="119">
       <c r="A119" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E119" s="0" t="n">
         <v>200127</v>
@@ -1914,7 +1928,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="120">
       <c r="A120" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E120" s="0" t="n">
         <v>200128</v>
@@ -1925,7 +1939,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="121">
       <c r="A121" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E121" s="0" t="n">
         <v>200129</v>
@@ -1936,7 +1950,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="122">
       <c r="A122" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E122" s="0" t="n">
         <v>200130</v>
@@ -1947,7 +1961,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="123">
       <c r="A123" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E123" s="0" t="n">
         <v>200131</v>
@@ -1958,7 +1972,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="124">
       <c r="A124" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E124" s="0" t="n">
         <v>200132</v>
@@ -1969,7 +1983,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="125">
       <c r="A125" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E125" s="0" t="n">
         <v>200133</v>
@@ -1980,7 +1994,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="126">
       <c r="A126" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E126" s="0" t="n">
         <v>200134</v>
@@ -1991,7 +2005,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="127">
       <c r="A127" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E127" s="0" t="n">
         <v>200135</v>
@@ -2002,7 +2016,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="128">
       <c r="A128" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E128" s="0" t="n">
         <v>200136</v>
@@ -2013,7 +2027,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="129">
       <c r="A129" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E129" s="0" t="n">
         <v>200137</v>
@@ -2024,7 +2038,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="130">
       <c r="A130" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E130" s="0" t="n">
         <v>200138</v>
@@ -2035,7 +2049,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="131">
       <c r="A131" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E131" s="0" t="n">
         <v>200139</v>
@@ -2046,7 +2060,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="132">
       <c r="A132" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E132" s="0" t="n">
         <v>200140</v>
@@ -2057,7 +2071,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="133">
       <c r="A133" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E133" s="0" t="n">
         <v>200141</v>
@@ -2068,7 +2082,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="134">
       <c r="A134" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E134" s="0" t="n">
         <v>200142</v>
@@ -2079,7 +2093,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="135">
       <c r="A135" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E135" s="0" t="n">
         <v>200143</v>
@@ -2090,7 +2104,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="136">
       <c r="A136" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E136" s="0" t="n">
         <v>200144</v>
@@ -2101,7 +2115,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="137">
       <c r="A137" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E137" s="0" t="n">
         <v>200145</v>
@@ -2112,7 +2126,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="138">
       <c r="A138" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E138" s="0" t="n">
         <v>200146</v>
@@ -2123,7 +2137,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="139">
       <c r="A139" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E139" s="0" t="n">
         <v>200147</v>
@@ -2134,7 +2148,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="140">
       <c r="A140" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E140" s="0" t="n">
         <v>200148</v>
@@ -2145,7 +2159,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="141">
       <c r="A141" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E141" s="0" t="n">
         <v>200149</v>
@@ -2156,7 +2170,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="142">
       <c r="A142" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E142" s="0" t="n">
         <v>200150</v>
@@ -2167,7 +2181,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="143">
       <c r="A143" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E143" s="0" t="n">
         <v>200151</v>
@@ -2178,7 +2192,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="144">
       <c r="A144" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E144" s="0" t="n">
         <v>200152</v>
@@ -2189,7 +2203,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="145">
       <c r="A145" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E145" s="0" t="n">
         <v>200153</v>
@@ -2200,7 +2214,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="146">
       <c r="A146" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E146" s="0" t="n">
         <v>200154</v>
@@ -2211,7 +2225,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="147">
       <c r="A147" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E147" s="0" t="n">
         <v>200155</v>
@@ -2222,7 +2236,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="148">
       <c r="A148" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E148" s="0" t="n">
         <v>200156</v>
@@ -2233,7 +2247,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="149">
       <c r="A149" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E149" s="0" t="n">
         <v>200157</v>
@@ -2244,7 +2258,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="150">
       <c r="A150" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E150" s="0" t="n">
         <v>200158</v>
@@ -2255,7 +2269,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="151">
       <c r="A151" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E151" s="0" t="n">
         <v>200159</v>
@@ -2266,7 +2280,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="152">
       <c r="A152" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E152" s="0" t="n">
         <v>200160</v>
@@ -2277,7 +2291,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="153">
       <c r="A153" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E153" s="0" t="n">
         <v>200161</v>
@@ -2288,7 +2302,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="154">
       <c r="A154" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E154" s="0" t="n">
         <v>200162</v>
@@ -2299,7 +2313,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="155">
       <c r="A155" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E155" s="0" t="n">
         <v>200163</v>
@@ -2310,7 +2324,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="156">
       <c r="A156" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E156" s="0" t="n">
         <v>200164</v>
@@ -2321,7 +2335,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="157">
       <c r="A157" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E157" s="0" t="n">
         <v>200165</v>
@@ -2332,7 +2346,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="158">
       <c r="A158" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E158" s="0" t="n">
         <v>200166</v>
@@ -2343,7 +2357,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="159">
       <c r="A159" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E159" s="0" t="n">
         <v>200167</v>
@@ -2354,7 +2368,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="160">
       <c r="A160" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E160" s="0" t="n">
         <v>200168</v>
@@ -2365,7 +2379,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="161">
       <c r="A161" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E161" s="0" t="n">
         <v>200169</v>
@@ -2376,7 +2390,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="162">
       <c r="A162" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E162" s="0" t="n">
         <v>200170</v>
@@ -2387,7 +2401,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="163">
       <c r="A163" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E163" s="0" t="n">
         <v>200171</v>
@@ -2398,7 +2412,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="164">
       <c r="A164" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E164" s="0" t="n">
         <v>200172</v>
@@ -2409,7 +2423,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="165">
       <c r="A165" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E165" s="0" t="n">
         <v>200173</v>
@@ -2420,7 +2434,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="166">
       <c r="A166" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E166" s="0" t="n">
         <v>200174</v>
@@ -2431,7 +2445,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="167">
       <c r="A167" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E167" s="0" t="n">
         <v>200175</v>
@@ -2442,7 +2456,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="168">
       <c r="A168" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E168" s="0" t="n">
         <v>200176</v>
@@ -2453,7 +2467,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="169">
       <c r="A169" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E169" s="0" t="n">
         <v>200177</v>
@@ -2464,7 +2478,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="170">
       <c r="A170" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E170" s="0" t="n">
         <v>200178</v>
@@ -2475,7 +2489,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="171">
       <c r="A171" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E171" s="0" t="n">
         <v>200179</v>
@@ -2486,7 +2500,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="172">
       <c r="A172" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E172" s="0" t="n">
         <v>200180</v>
@@ -2497,7 +2511,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="173">
       <c r="A173" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E173" s="0" t="n">
         <v>200181</v>
@@ -2508,7 +2522,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="174">
       <c r="A174" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E174" s="0" t="n">
         <v>200182</v>
@@ -2519,7 +2533,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="175">
       <c r="A175" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E175" s="0" t="n">
         <v>200183</v>
@@ -2530,7 +2544,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="176">
       <c r="A176" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E176" s="0" t="n">
         <v>200184</v>
@@ -2541,7 +2555,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="177">
       <c r="A177" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E177" s="0" t="n">
         <v>200185</v>
@@ -2552,7 +2566,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="178">
       <c r="A178" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E178" s="0" t="n">
         <v>200186</v>
@@ -2563,7 +2577,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="179">
       <c r="A179" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E179" s="0" t="n">
         <v>200187</v>
@@ -2574,7 +2588,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="180">
       <c r="A180" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E180" s="0" t="n">
         <v>200188</v>
@@ -2585,7 +2599,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="181">
       <c r="A181" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E181" s="0" t="n">
         <v>200189</v>
@@ -2596,7 +2610,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="182">
       <c r="A182" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E182" s="0" t="n">
         <v>200190</v>
@@ -2607,7 +2621,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="183">
       <c r="A183" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E183" s="0" t="n">
         <v>200191</v>
@@ -2618,7 +2632,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="184">
       <c r="A184" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E184" s="0" t="n">
         <v>200192</v>
@@ -2629,7 +2643,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="185">
       <c r="A185" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E185" s="0" t="n">
         <v>200193</v>
@@ -2640,7 +2654,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="186">
       <c r="A186" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E186" s="0" t="n">
         <v>200194</v>
@@ -2651,7 +2665,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="187">
       <c r="A187" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E187" s="0" t="n">
         <v>200195</v>
@@ -2662,7 +2676,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="188">
       <c r="A188" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E188" s="0" t="n">
         <v>200196</v>
@@ -2673,7 +2687,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="189">
       <c r="A189" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E189" s="0" t="n">
         <v>200197</v>
@@ -2684,7 +2698,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="190">
       <c r="A190" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E190" s="0" t="n">
         <v>200198</v>
@@ -2695,7 +2709,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="191">
       <c r="A191" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E191" s="0" t="n">
         <v>200199</v>
@@ -2706,7 +2720,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="192">
       <c r="A192" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E192" s="0" t="n">
         <v>200200</v>
@@ -2717,7 +2731,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="193">
       <c r="A193" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E193" s="0" t="n">
         <v>200201</v>
@@ -2728,7 +2742,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="194">
       <c r="A194" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E194" s="0" t="n">
         <v>200202</v>
@@ -2739,7 +2753,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="195">
       <c r="A195" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E195" s="0" t="n">
         <v>200203</v>
@@ -2750,7 +2764,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="196">
       <c r="A196" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E196" s="0" t="n">
         <v>200204</v>
@@ -2761,7 +2775,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="197">
       <c r="A197" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E197" s="0" t="n">
         <v>200207</v>
@@ -2772,7 +2786,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="198">
       <c r="A198" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E198" s="0" t="n">
         <v>200209</v>
@@ -2783,7 +2797,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="199">
       <c r="A199" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E199" s="0" t="n">
         <v>200211</v>
@@ -2794,7 +2808,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="200">
       <c r="A200" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E200" s="0" t="n">
         <v>200212</v>
@@ -2805,7 +2819,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="201">
       <c r="A201" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E201" s="0" t="n">
         <v>200213</v>
@@ -2816,7 +2830,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="202">
       <c r="A202" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E202" s="0" t="n">
         <v>200214</v>
@@ -2827,7 +2841,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="203">
       <c r="A203" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E203" s="0" t="n">
         <v>200215</v>
@@ -2838,7 +2852,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="204">
       <c r="A204" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E204" s="0" t="n">
         <v>200216</v>
@@ -2849,7 +2863,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="205">
       <c r="A205" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E205" s="0" t="n">
         <v>200217</v>
@@ -2860,7 +2874,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="206">
       <c r="A206" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E206" s="0" t="n">
         <v>200218</v>
@@ -2871,7 +2885,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="207">
       <c r="A207" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E207" s="0" t="n">
         <v>200219</v>
@@ -2882,7 +2896,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="208">
       <c r="A208" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E208" s="0" t="n">
         <v>200220</v>
@@ -2893,7 +2907,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="209">
       <c r="A209" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E209" s="0" t="n">
         <v>200221</v>
@@ -2904,7 +2918,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="210">
       <c r="A210" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E210" s="0" t="n">
         <v>200222</v>
@@ -2915,7 +2929,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="211">
       <c r="A211" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E211" s="0" t="n">
         <v>200223</v>
@@ -2926,7 +2940,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="212">
       <c r="A212" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E212" s="0" t="n">
         <v>200224</v>
@@ -2937,7 +2951,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="213">
       <c r="A213" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E213" s="0" t="n">
         <v>200225</v>
@@ -2948,7 +2962,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="214">
       <c r="A214" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E214" s="0" t="n">
         <v>200226</v>
@@ -2959,7 +2973,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="215">
       <c r="A215" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E215" s="0" t="n">
         <v>200227</v>
@@ -2970,7 +2984,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="216">
       <c r="A216" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E216" s="0" t="n">
         <v>200228</v>
@@ -2981,7 +2995,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="217">
       <c r="A217" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E217" s="0" t="n">
         <v>200229</v>
@@ -2992,7 +3006,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="218">
       <c r="A218" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E218" s="0" t="n">
         <v>200230</v>
@@ -3003,7 +3017,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="219">
       <c r="A219" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E219" s="0" t="n">
         <v>200231</v>
@@ -3014,7 +3028,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="220">
       <c r="A220" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E220" s="0" t="n">
         <v>200232</v>
@@ -3025,7 +3039,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="221">
       <c r="A221" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E221" s="0" t="n">
         <v>200233</v>
@@ -3036,7 +3050,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="222">
       <c r="A222" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E222" s="0" t="n">
         <v>200234</v>
@@ -3047,7 +3061,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="223">
       <c r="A223" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E223" s="0" t="n">
         <v>200235</v>
@@ -3058,7 +3072,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="224">
       <c r="A224" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E224" s="0" t="n">
         <v>200236</v>
@@ -3069,7 +3083,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="225">
       <c r="A225" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E225" s="0" t="n">
         <v>200237</v>
@@ -3080,7 +3094,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="226">
       <c r="A226" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E226" s="0" t="n">
         <v>200238</v>
@@ -3091,7 +3105,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="227">
       <c r="A227" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E227" s="0" t="n">
         <v>200239</v>
@@ -3102,7 +3116,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="228">
       <c r="A228" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E228" s="0" t="n">
         <v>200240</v>
@@ -3113,7 +3127,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="229">
       <c r="A229" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E229" s="0" t="n">
         <v>200241</v>
@@ -3124,7 +3138,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="230">
       <c r="A230" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E230" s="0" t="n">
         <v>200242</v>
@@ -3135,7 +3149,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="231">
       <c r="A231" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E231" s="0" t="n">
         <v>200243</v>
@@ -3146,7 +3160,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="232">
       <c r="A232" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E232" s="0" t="n">
         <v>200244</v>
@@ -3157,7 +3171,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="233">
       <c r="A233" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E233" s="0" t="n">
         <v>200245</v>
@@ -3168,7 +3182,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="234">
       <c r="A234" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E234" s="0" t="n">
         <v>200246</v>
@@ -3179,7 +3193,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="235">
       <c r="A235" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E235" s="0" t="n">
         <v>200247</v>
@@ -3190,7 +3204,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="236">
       <c r="A236" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E236" s="0" t="n">
         <v>200248</v>
@@ -3201,7 +3215,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="237">
       <c r="A237" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E237" s="0" t="n">
         <v>200249</v>
@@ -3212,7 +3226,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="238">
       <c r="A238" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E238" s="0" t="n">
         <v>200250</v>
@@ -3223,7 +3237,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="239">
       <c r="A239" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E239" s="0" t="n">
         <v>200251</v>
@@ -3234,7 +3248,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="240">
       <c r="A240" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E240" s="0" t="n">
         <v>200252</v>
@@ -3245,7 +3259,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="241">
       <c r="A241" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E241" s="0" t="n">
         <v>200253</v>
@@ -3256,7 +3270,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="242">
       <c r="A242" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E242" s="0" t="n">
         <v>200254</v>
@@ -3267,7 +3281,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="243">
       <c r="A243" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E243" s="0" t="n">
         <v>200255</v>
@@ -3278,7 +3292,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="244">
       <c r="A244" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E244" s="0" t="n">
         <v>200256</v>
@@ -3289,7 +3303,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="245">
       <c r="A245" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E245" s="0" t="n">
         <v>200257</v>
@@ -3300,7 +3314,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="246">
       <c r="A246" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E246" s="0" t="n">
         <v>200258</v>
@@ -3311,7 +3325,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="247">
       <c r="A247" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E247" s="0" t="n">
         <v>200259</v>
@@ -3322,7 +3336,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="248">
       <c r="A248" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E248" s="0" t="n">
         <v>200260</v>
@@ -3333,7 +3347,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="249">
       <c r="A249" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E249" s="0" t="n">
         <v>200261</v>
@@ -3344,7 +3358,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="250">
       <c r="A250" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E250" s="0" t="n">
         <v>200262</v>
@@ -3355,7 +3369,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="251">
       <c r="A251" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E251" s="0" t="n">
         <v>200263</v>
@@ -3366,7 +3380,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="252">
       <c r="A252" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E252" s="0" t="n">
         <v>200264</v>
@@ -3377,7 +3391,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="253">
       <c r="A253" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E253" s="0" t="n">
         <v>200265</v>
@@ -3388,7 +3402,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="254">
       <c r="A254" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E254" s="0" t="n">
         <v>200266</v>
@@ -3399,7 +3413,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="255">
       <c r="A255" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E255" s="0" t="n">
         <v>200267</v>
@@ -3410,7 +3424,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="256">
       <c r="A256" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E256" s="0" t="n">
         <v>200268</v>
@@ -3421,7 +3435,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="257">
       <c r="A257" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E257" s="0" t="n">
         <v>200269</v>
@@ -3432,7 +3446,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="258">
       <c r="A258" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E258" s="0" t="n">
         <v>200270</v>
@@ -3443,7 +3457,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="259">
       <c r="A259" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E259" s="0" t="n">
         <v>200271</v>
@@ -3454,7 +3468,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="260">
       <c r="A260" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E260" s="0" t="n">
         <v>200272</v>
@@ -3465,7 +3479,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="261">
       <c r="A261" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E261" s="0" t="n">
         <v>200273</v>
@@ -3476,7 +3490,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="262">
       <c r="A262" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E262" s="0" t="n">
         <v>200274</v>
@@ -3487,7 +3501,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="263">
       <c r="A263" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E263" s="0" t="n">
         <v>200275</v>
@@ -3498,7 +3512,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="264">
       <c r="A264" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E264" s="0" t="n">
         <v>200276</v>
@@ -3509,7 +3523,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="265">
       <c r="A265" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E265" s="0" t="n">
         <v>200277</v>
@@ -3520,7 +3534,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="266">
       <c r="A266" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E266" s="0" t="n">
         <v>200278</v>
@@ -3531,7 +3545,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="267">
       <c r="A267" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E267" s="0" t="n">
         <v>200279</v>
@@ -3542,7 +3556,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="268">
       <c r="A268" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E268" s="0" t="n">
         <v>200280</v>
@@ -3553,7 +3567,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="269">
       <c r="A269" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E269" s="0" t="n">
         <v>200281</v>
@@ -3564,7 +3578,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="270">
       <c r="A270" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E270" s="0" t="n">
         <v>200282</v>
@@ -3575,7 +3589,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="271">
       <c r="A271" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E271" s="0" t="n">
         <v>200283</v>
@@ -3586,7 +3600,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="272">
       <c r="A272" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E272" s="0" t="n">
         <v>200284</v>
@@ -3597,7 +3611,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="273">
       <c r="A273" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E273" s="0" t="n">
         <v>200285</v>
@@ -3608,7 +3622,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="274">
       <c r="A274" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E274" s="0" t="n">
         <v>200286</v>
@@ -3619,7 +3633,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="275">
       <c r="A275" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E275" s="0" t="n">
         <v>200287</v>
@@ -3630,7 +3644,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="276">
       <c r="A276" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E276" s="0" t="n">
         <v>200288</v>
@@ -3641,7 +3655,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="277">
       <c r="A277" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E277" s="0" t="n">
         <v>200289</v>
@@ -3652,7 +3666,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="278">
       <c r="A278" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E278" s="0" t="n">
         <v>200290</v>
@@ -3663,7 +3677,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="279">
       <c r="A279" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E279" s="0" t="n">
         <v>200291</v>
@@ -3674,7 +3688,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="280">
       <c r="A280" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E280" s="0" t="n">
         <v>200292</v>
@@ -3685,7 +3699,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="281">
       <c r="A281" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E281" s="0" t="n">
         <v>200293</v>
@@ -3696,7 +3710,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="282">
       <c r="A282" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E282" s="0" t="n">
         <v>200294</v>
@@ -3707,7 +3721,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="283">
       <c r="A283" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E283" s="0" t="n">
         <v>200295</v>
@@ -3718,7 +3732,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="284">
       <c r="A284" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E284" s="0" t="n">
         <v>200296</v>
@@ -3729,7 +3743,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="285">
       <c r="A285" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E285" s="0" t="n">
         <v>200297</v>
@@ -3740,7 +3754,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="286">
       <c r="A286" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E286" s="0" t="n">
         <v>200298</v>
@@ -3751,7 +3765,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="287">
       <c r="A287" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E287" s="0" t="n">
         <v>200299</v>
@@ -3762,7 +3776,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="288">
       <c r="A288" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E288" s="0" t="n">
         <v>200300</v>
@@ -3773,7 +3787,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="289">
       <c r="A289" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E289" s="0" t="n">
         <v>200301</v>
@@ -3784,7 +3798,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="290">
       <c r="A290" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E290" s="0" t="n">
         <v>200302</v>
@@ -3795,7 +3809,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="291">
       <c r="A291" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E291" s="0" t="n">
         <v>200303</v>
@@ -3806,7 +3820,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="292">
       <c r="A292" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E292" s="0" t="n">
         <v>200304</v>
@@ -3817,7 +3831,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="293">
       <c r="A293" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E293" s="0" t="n">
         <v>200305</v>
@@ -3828,7 +3842,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="294">
       <c r="A294" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E294" s="0" t="n">
         <v>200306</v>
@@ -3839,7 +3853,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="295">
       <c r="A295" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E295" s="0" t="n">
         <v>200307</v>
@@ -3850,7 +3864,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="296">
       <c r="A296" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E296" s="0" t="n">
         <v>200309</v>
@@ -3861,7 +3875,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="297">
       <c r="A297" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E297" s="0" t="n">
         <v>200310</v>
@@ -3872,7 +3886,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="298">
       <c r="A298" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E298" s="0" t="n">
         <v>200311</v>
@@ -3883,7 +3897,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="299">
       <c r="A299" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E299" s="0" t="n">
         <v>200312</v>
@@ -3894,7 +3908,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="300">
       <c r="A300" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E300" s="0" t="n">
         <v>200313</v>
@@ -3905,7 +3919,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="301">
       <c r="A301" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E301" s="0" t="n">
         <v>200314</v>
@@ -3916,7 +3930,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="302">
       <c r="A302" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E302" s="0" t="n">
         <v>200315</v>
@@ -3927,7 +3941,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="303">
       <c r="A303" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E303" s="0" t="n">
         <v>200316</v>
@@ -3938,7 +3952,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="304">
       <c r="A304" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E304" s="0" t="n">
         <v>200317</v>
@@ -3949,7 +3963,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="305">
       <c r="A305" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E305" s="0" t="n">
         <v>200318</v>
@@ -3960,7 +3974,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="306">
       <c r="A306" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E306" s="0" t="n">
         <v>200319</v>
@@ -3971,7 +3985,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="307">
       <c r="A307" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E307" s="0" t="n">
         <v>200320</v>
@@ -3982,7 +3996,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="308">
       <c r="A308" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E308" s="0" t="n">
         <v>200321</v>
@@ -3993,7 +4007,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="309">
       <c r="A309" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E309" s="0" t="n">
         <v>200322</v>
@@ -4004,7 +4018,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="310">
       <c r="A310" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E310" s="0" t="n">
         <v>200323</v>
@@ -4015,7 +4029,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="311">
       <c r="A311" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E311" s="0" t="n">
         <v>200324</v>
@@ -4026,7 +4040,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="312">
       <c r="A312" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E312" s="0" t="n">
         <v>200325</v>
@@ -4037,7 +4051,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="313">
       <c r="A313" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E313" s="0" t="n">
         <v>200326</v>
@@ -4048,7 +4062,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="314">
       <c r="A314" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E314" s="0" t="n">
         <v>200327</v>
@@ -4059,7 +4073,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="315">
       <c r="A315" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E315" s="0" t="n">
         <v>200328</v>
@@ -4070,7 +4084,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="316">
       <c r="A316" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E316" s="0" t="n">
         <v>200329</v>
@@ -4081,7 +4095,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="317">
       <c r="A317" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E317" s="0" t="n">
         <v>200330</v>
@@ -4092,7 +4106,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="318">
       <c r="A318" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E318" s="0" t="n">
         <v>200331</v>
@@ -4103,7 +4117,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="319">
       <c r="A319" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E319" s="0" t="n">
         <v>200332</v>
@@ -4114,7 +4128,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="320">
       <c r="A320" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E320" s="0" t="n">
         <v>200333</v>
@@ -4125,7 +4139,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="321">
       <c r="A321" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E321" s="0" t="n">
         <v>200334</v>
@@ -4136,7 +4150,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="322">
       <c r="A322" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E322" s="0" t="n">
         <v>200335</v>
@@ -4147,7 +4161,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="323">
       <c r="A323" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E323" s="0" t="n">
         <v>200336</v>
@@ -4158,7 +4172,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="324">
       <c r="A324" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E324" s="0" t="n">
         <v>200337</v>
@@ -4169,7 +4183,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="325">
       <c r="A325" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E325" s="0" t="n">
         <v>200338</v>
@@ -4180,7 +4194,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="326">
       <c r="A326" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E326" s="0" t="n">
         <v>200339</v>
@@ -4191,7 +4205,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="327">
       <c r="A327" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E327" s="0" t="n">
         <v>200340</v>
@@ -4202,7 +4216,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="328">
       <c r="A328" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E328" s="0" t="n">
         <v>200341</v>
@@ -4213,7 +4227,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="329">
       <c r="A329" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E329" s="0" t="n">
         <v>200342</v>
@@ -4224,7 +4238,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="330">
       <c r="A330" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E330" s="0" t="n">
         <v>200343</v>
@@ -4235,7 +4249,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="331">
       <c r="A331" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E331" s="0" t="n">
         <v>200344</v>
@@ -4246,7 +4260,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="332">
       <c r="A332" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E332" s="0" t="n">
         <v>200345</v>
@@ -4257,7 +4271,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="333">
       <c r="A333" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E333" s="0" t="n">
         <v>200346</v>
@@ -4268,7 +4282,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="334">
       <c r="A334" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E334" s="0" t="n">
         <v>200347</v>
@@ -4279,7 +4293,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="335">
       <c r="A335" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E335" s="0" t="n">
         <v>200348</v>
@@ -4290,7 +4304,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="336">
       <c r="A336" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E336" s="0" t="n">
         <v>200349</v>
@@ -4301,7 +4315,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="337">
       <c r="A337" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E337" s="0" t="n">
         <v>200350</v>
@@ -4312,7 +4326,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="338">
       <c r="A338" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E338" s="0" t="n">
         <v>200351</v>
@@ -4323,7 +4337,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="339">
       <c r="A339" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E339" s="0" t="n">
         <v>200352</v>
@@ -4334,7 +4348,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="340">
       <c r="A340" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E340" s="0" t="n">
         <v>200353</v>
@@ -4345,7 +4359,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="341">
       <c r="A341" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E341" s="0" t="n">
         <v>200354</v>
@@ -4356,7 +4370,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="342">
       <c r="A342" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E342" s="0" t="n">
         <v>200355</v>
@@ -4367,7 +4381,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="343">
       <c r="A343" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E343" s="0" t="n">
         <v>200356</v>
@@ -4378,7 +4392,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="344">
       <c r="A344" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E344" s="0" t="n">
         <v>200357</v>
@@ -4389,7 +4403,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="345">
       <c r="A345" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E345" s="0" t="n">
         <v>200358</v>
@@ -4400,7 +4414,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="346">
       <c r="A346" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E346" s="0" t="n">
         <v>200359</v>
@@ -4411,7 +4425,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="347">
       <c r="A347" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E347" s="0" t="n">
         <v>200360</v>
@@ -4422,7 +4436,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="348">
       <c r="A348" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E348" s="0" t="n">
         <v>200361</v>
@@ -4433,7 +4447,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="349">
       <c r="A349" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E349" s="0" t="n">
         <v>200362</v>
@@ -4444,7 +4458,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="350">
       <c r="A350" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E350" s="0" t="n">
         <v>200363</v>
@@ -4455,7 +4469,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="351">
       <c r="A351" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E351" s="0" t="n">
         <v>200364</v>
@@ -4466,7 +4480,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="352">
       <c r="A352" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E352" s="0" t="n">
         <v>200365</v>
@@ -4477,7 +4491,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="353">
       <c r="A353" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E353" s="0" t="n">
         <v>200366</v>
@@ -4488,7 +4502,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="354">
       <c r="A354" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E354" s="0" t="n">
         <v>200367</v>
@@ -4499,7 +4513,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="355">
       <c r="A355" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E355" s="0" t="n">
         <v>200368</v>
@@ -4510,7 +4524,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="356">
       <c r="A356" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E356" s="0" t="n">
         <v>200369</v>
@@ -4521,7 +4535,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="357">
       <c r="A357" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E357" s="0" t="n">
         <v>200370</v>
@@ -4532,7 +4546,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="358">
       <c r="A358" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E358" s="0" t="n">
         <v>200371</v>
@@ -4543,7 +4557,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="359">
       <c r="A359" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E359" s="0" t="n">
         <v>200372</v>
@@ -4554,7 +4568,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="360">
       <c r="A360" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E360" s="0" t="n">
         <v>200373</v>
@@ -4565,7 +4579,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="361">
       <c r="A361" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E361" s="0" t="n">
         <v>200374</v>
@@ -4576,7 +4590,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="362">
       <c r="A362" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E362" s="0" t="n">
         <v>200375</v>
@@ -4587,7 +4601,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="363">
       <c r="A363" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E363" s="0" t="n">
         <v>200376</v>
@@ -4598,7 +4612,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="364">
       <c r="A364" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E364" s="0" t="n">
         <v>200377</v>
@@ -4609,7 +4623,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="365">
       <c r="A365" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E365" s="0" t="n">
         <v>200378</v>
@@ -4620,7 +4634,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="366">
       <c r="A366" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E366" s="0" t="n">
         <v>200379</v>
@@ -4631,7 +4645,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="367">
       <c r="A367" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E367" s="0" t="n">
         <v>200380</v>
@@ -4642,7 +4656,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="368">
       <c r="A368" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E368" s="0" t="n">
         <v>200381</v>
@@ -4653,7 +4667,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="369">
       <c r="A369" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E369" s="0" t="n">
         <v>200382</v>
@@ -4664,7 +4678,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="370">
       <c r="A370" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E370" s="0" t="n">
         <v>200383</v>
@@ -4675,7 +4689,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="371">
       <c r="A371" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E371" s="0" t="n">
         <v>200390</v>
@@ -4686,7 +4700,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="372">
       <c r="A372" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E372" s="0" t="n">
         <v>200392</v>
@@ -4697,7 +4711,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="373">
       <c r="A373" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E373" s="0" t="n">
         <v>200394</v>
@@ -4708,7 +4722,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="374">
       <c r="A374" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E374" s="0" t="n">
         <v>200396</v>
@@ -4719,7 +4733,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="375">
       <c r="A375" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E375" s="0" t="n">
         <v>200399</v>
@@ -4730,7 +4744,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="376">
       <c r="A376" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E376" s="0" t="n">
         <v>200400</v>
@@ -4741,7 +4755,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="377">
       <c r="A377" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E377" s="0" t="n">
         <v>200401</v>
@@ -4752,7 +4766,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="378">
       <c r="A378" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E378" s="0" t="n">
         <v>200402</v>
@@ -4763,7 +4777,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="379">
       <c r="A379" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E379" s="0" t="n">
         <v>200403</v>
@@ -4774,7 +4788,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="380">
       <c r="A380" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E380" s="0" t="n">
         <v>200404</v>
@@ -4785,7 +4799,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="381">
       <c r="A381" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E381" s="0" t="n">
         <v>200405</v>
@@ -4796,7 +4810,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="382">
       <c r="A382" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E382" s="0" t="n">
         <v>200406</v>
@@ -4807,7 +4821,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="383">
       <c r="A383" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E383" s="0" t="n">
         <v>200407</v>
@@ -4818,7 +4832,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="384">
       <c r="A384" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E384" s="0" t="n">
         <v>200408</v>
@@ -4829,7 +4843,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="385">
       <c r="A385" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E385" s="0" t="n">
         <v>200409</v>
@@ -4840,7 +4854,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="386">
       <c r="A386" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E386" s="0" t="n">
         <v>200410</v>
@@ -4851,7 +4865,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="387">
       <c r="A387" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E387" s="0" t="n">
         <v>200411</v>
@@ -4862,7 +4876,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="388">
       <c r="A388" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E388" s="0" t="n">
         <v>200412</v>
@@ -4873,7 +4887,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="389">
       <c r="A389" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E389" s="0" t="n">
         <v>200413</v>
@@ -4884,7 +4898,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="390">
       <c r="A390" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E390" s="0" t="n">
         <v>200414</v>
@@ -4895,7 +4909,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="391">
       <c r="A391" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E391" s="0" t="n">
         <v>200415</v>
@@ -4906,7 +4920,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="392">
       <c r="A392" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E392" s="0" t="n">
         <v>200416</v>
@@ -4917,7 +4931,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="393">
       <c r="A393" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E393" s="0" t="n">
         <v>200417</v>
@@ -4928,7 +4942,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="394">
       <c r="A394" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E394" s="0" t="n">
         <v>200418</v>
@@ -4939,7 +4953,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="395">
       <c r="A395" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E395" s="0" t="n">
         <v>200419</v>
@@ -4950,7 +4964,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="396">
       <c r="A396" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E396" s="0" t="n">
         <v>200420</v>
@@ -4961,7 +4975,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="397">
       <c r="A397" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E397" s="0" t="n">
         <v>200421</v>
@@ -4972,7 +4986,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="398">
       <c r="A398" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E398" s="0" t="n">
         <v>200422</v>
@@ -4983,7 +4997,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="399">
       <c r="A399" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E399" s="0" t="n">
         <v>200423</v>
@@ -4994,7 +5008,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="400">
       <c r="A400" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E400" s="0" t="n">
         <v>200424</v>
@@ -5005,7 +5019,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="401">
       <c r="A401" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E401" s="0" t="n">
         <v>200425</v>
@@ -5016,7 +5030,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="402">
       <c r="A402" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E402" s="0" t="n">
         <v>200426</v>
@@ -5027,7 +5041,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="403">
       <c r="A403" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E403" s="0" t="n">
         <v>200427</v>
@@ -5038,7 +5052,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="404">
       <c r="A404" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E404" s="0" t="n">
         <v>200428</v>
@@ -5049,7 +5063,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="405">
       <c r="A405" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E405" s="0" t="n">
         <v>200429</v>
@@ -5060,7 +5074,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="406">
       <c r="A406" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E406" s="0" t="n">
         <v>200430</v>
@@ -5071,7 +5085,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="407">
       <c r="A407" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E407" s="0" t="n">
         <v>200431</v>
@@ -5082,7 +5096,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="408">
       <c r="A408" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E408" s="0" t="n">
         <v>200432</v>
@@ -5093,7 +5107,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="409">
       <c r="A409" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E409" s="0" t="n">
         <v>200433</v>
@@ -5104,7 +5118,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="410">
       <c r="A410" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E410" s="0" t="n">
         <v>200434</v>
@@ -5115,7 +5129,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="411">
       <c r="A411" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E411" s="0" t="n">
         <v>200435</v>
@@ -5126,7 +5140,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="412">
       <c r="A412" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E412" s="0" t="n">
         <v>200436</v>
@@ -5137,7 +5151,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="413">
       <c r="A413" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E413" s="0" t="n">
         <v>200437</v>
@@ -5148,7 +5162,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="414">
       <c r="A414" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E414" s="0" t="n">
         <v>200438</v>
@@ -5159,7 +5173,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="415">
       <c r="A415" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E415" s="0" t="n">
         <v>200439</v>
@@ -5170,7 +5184,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="416">
       <c r="A416" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E416" s="0" t="n">
         <v>200440</v>
@@ -5181,7 +5195,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="417">
       <c r="A417" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E417" s="0" t="n">
         <v>200441</v>
@@ -5192,7 +5206,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="418">
       <c r="A418" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E418" s="0" t="n">
         <v>200442</v>
@@ -5203,7 +5217,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="419">
       <c r="A419" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E419" s="0" t="n">
         <v>200443</v>
@@ -5214,7 +5228,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="420">
       <c r="A420" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E420" s="0" t="n">
         <v>200444</v>
@@ -5225,7 +5239,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="421">
       <c r="A421" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E421" s="0" t="n">
         <v>200445</v>
@@ -5236,7 +5250,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="422">
       <c r="A422" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E422" s="0" t="n">
         <v>200446</v>
@@ -5247,7 +5261,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="423">
       <c r="A423" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E423" s="0" t="n">
         <v>200447</v>
@@ -5258,7 +5272,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="424">
       <c r="A424" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E424" s="0" t="n">
         <v>200448</v>
@@ -5269,7 +5283,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="425">
       <c r="A425" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E425" s="0" t="n">
         <v>200449</v>
@@ -5280,7 +5294,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="426">
       <c r="A426" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E426" s="0" t="n">
         <v>200450</v>
@@ -5291,7 +5305,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="427">
       <c r="A427" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E427" s="0" t="n">
         <v>200451</v>
@@ -5302,7 +5316,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="428">
       <c r="A428" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E428" s="0" t="n">
         <v>200454</v>
@@ -5313,7 +5327,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="429">
       <c r="A429" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E429" s="0" t="n">
         <v>200455</v>
@@ -5324,7 +5338,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="430">
       <c r="A430" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E430" s="0" t="n">
         <v>200456</v>
@@ -5335,7 +5349,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="431">
       <c r="A431" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E431" s="0" t="n">
         <v>200457</v>
@@ -5346,7 +5360,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="432">
       <c r="A432" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E432" s="0" t="n">
         <v>200458</v>
@@ -5357,7 +5371,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="433">
       <c r="A433" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E433" s="0" t="n">
         <v>200459</v>
@@ -5368,7 +5382,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="434">
       <c r="A434" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E434" s="0" t="n">
         <v>200460</v>
@@ -5379,7 +5393,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="435">
       <c r="A435" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E435" s="0" t="n">
         <v>200461</v>
@@ -5390,7 +5404,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="436">
       <c r="A436" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E436" s="0" t="n">
         <v>200462</v>
@@ -5401,7 +5415,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="437">
       <c r="A437" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E437" s="0" t="n">
         <v>200463</v>
@@ -5412,7 +5426,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="438">
       <c r="A438" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E438" s="0" t="n">
         <v>200464</v>
@@ -5423,7 +5437,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="439">
       <c r="A439" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E439" s="0" t="n">
         <v>200465</v>
@@ -5434,7 +5448,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="440">
       <c r="A440" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E440" s="0" t="n">
         <v>200466</v>
@@ -5445,7 +5459,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="441">
       <c r="A441" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E441" s="0" t="n">
         <v>200467</v>
@@ -5456,7 +5470,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="442">
       <c r="A442" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E442" s="0" t="n">
         <v>200468</v>
@@ -5467,7 +5481,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="443">
       <c r="A443" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E443" s="0" t="n">
         <v>200469</v>

</xml_diff>

<commit_message>
add new fields for #213, #214, #215
</commit_message>
<xml_diff>
--- a/sampledata/Screen20020_HMSL10008_kinomescan.xlsx
+++ b/sampledata/Screen20020_HMSL10008_kinomescan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="61">
   <si>
     <t>Field</t>
   </si>
@@ -116,6 +116,12 @@
     <t>Date Publicly Available</t>
   </si>
   <si>
+    <t>Most Recent Update</t>
+  </si>
+  <si>
+    <t>2014-01-03</t>
+  </si>
+  <si>
     <t>Is Restricted</t>
   </si>
   <si>
@@ -123,6 +129,9 @@
   </si>
   <si>
     <t>KINOMEscan</t>
+  </si>
+  <si>
+    <t>Bioassay</t>
   </si>
   <si>
     <t>"Data" Worksheet Column</t>
@@ -216,7 +225,7 @@
       <name val="Arial"/>
       <charset val="1"/>
       <family val="2"/>
-      <color rgb="00000000"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
     </font>
     <font>
@@ -277,15 +286,30 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+  <cellXfs count="7">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
@@ -308,22 +332,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B17" activeCellId="0" pane="topLeft" sqref="B17"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A6" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A16" activeCellId="0" pane="topLeft" sqref="A16"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.6666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="163.16862745098"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="11.6666666666667"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="163.16862745098"/>
-    <col collapsed="false" hidden="false" max="513" min="259" style="1" width="11.6666666666667"/>
-    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="163.16862745098"/>
-    <col collapsed="false" hidden="false" max="769" min="515" style="1" width="11.6666666666667"/>
-    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="163.16862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="771" style="1" width="11.6666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.6734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="163.168367346939"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="11.6734693877551"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="163.168367346939"/>
+    <col collapsed="false" hidden="false" max="513" min="259" style="1" width="11.6734693877551"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="163.168367346939"/>
+    <col collapsed="false" hidden="false" max="769" min="515" style="1" width="11.6734693877551"/>
+    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="163.168367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="771" style="1" width="11.6734693877551"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -447,16 +472,33 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="19">
+      <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -481,92 +523,93 @@
       <selection activeCell="B8" activeCellId="0" pane="topLeft" sqref="B8"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.721568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.719387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.64795918367347"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="5" t="s">
-        <v>32</v>
+      <c r="A1" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="5" t="s">
-        <v>34</v>
+      <c r="A2" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
-      <c r="A3" s="5" t="s">
-        <v>36</v>
+      <c r="A3" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
-      <c r="A4" s="5" t="s">
-        <v>38</v>
+      <c r="A4" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="A5" s="5" t="s">
-        <v>40</v>
+      <c r="A5" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
-      <c r="A6" s="5" t="s">
-        <v>41</v>
+      <c r="A6" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="A7" s="5" t="s">
-        <v>42</v>
+      <c r="A7" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="A8" s="5" t="s">
-        <v>43</v>
+      <c r="A8" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="A9" s="5" t="s">
-        <v>44</v>
+      <c r="A9" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="A10" s="5" t="s">
-        <v>46</v>
+      <c r="A10" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
-      <c r="A11" s="5" t="s">
-        <v>47</v>
+      <c r="A11" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="A12" s="5" t="s">
-        <v>48</v>
+      <c r="A12" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
-      <c r="A13" s="5" t="s">
-        <v>49</v>
+      <c r="A13" s="6" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -591,46 +634,47 @@
       <selection activeCell="I1" activeCellId="0" pane="topLeft" sqref="I1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.643137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.38039215686275"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.71372549019608"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.15294117647059"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.07450980392157"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.556862745098"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.74117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.38265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.71428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.14795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.07142857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.73979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.64795918367347"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>200001</v>
@@ -641,7 +685,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>200004</v>
@@ -652,7 +696,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>200006</v>
@@ -663,7 +707,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>200007</v>
@@ -674,7 +718,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>200009</v>
@@ -685,7 +729,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>200010</v>
@@ -696,7 +740,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>200012</v>
@@ -707,7 +751,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>200013</v>
@@ -718,7 +762,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>200015</v>
@@ -729,7 +773,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>200017</v>
@@ -740,7 +784,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>200018</v>
@@ -751,7 +795,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>200020</v>
@@ -762,7 +806,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>200021</v>
@@ -773,7 +817,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>200023</v>
@@ -784,7 +828,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>200024</v>
@@ -795,7 +839,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>200025</v>
@@ -806,7 +850,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>200026</v>
@@ -817,7 +861,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>200027</v>
@@ -828,7 +872,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>200028</v>
@@ -839,7 +883,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>200029</v>
@@ -850,7 +894,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>200030</v>
@@ -861,7 +905,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>200031</v>
@@ -872,7 +916,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>200032</v>
@@ -883,7 +927,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>200033</v>
@@ -894,7 +938,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>200034</v>
@@ -905,7 +949,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>200035</v>
@@ -916,7 +960,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>200036</v>
@@ -927,7 +971,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>200037</v>
@@ -938,7 +982,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>200038</v>
@@ -949,7 +993,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>200039</v>
@@ -960,7 +1004,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>200040</v>
@@ -971,7 +1015,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>200041</v>
@@ -982,7 +1026,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>200042</v>
@@ -993,7 +1037,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>200043</v>
@@ -1004,7 +1048,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>200044</v>
@@ -1015,7 +1059,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>200045</v>
@@ -1026,7 +1070,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>200046</v>
@@ -1037,7 +1081,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>200047</v>
@@ -1048,7 +1092,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>200048</v>
@@ -1059,7 +1103,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>200049</v>
@@ -1070,7 +1114,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>200050</v>
@@ -1081,7 +1125,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>200051</v>
@@ -1092,7 +1136,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>200052</v>
@@ -1103,7 +1147,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>200053</v>
@@ -1114,7 +1158,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>200054</v>
@@ -1125,7 +1169,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>200055</v>
@@ -1136,7 +1180,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>200056</v>
@@ -1147,7 +1191,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>200057</v>
@@ -1158,7 +1202,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="A50" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>200058</v>
@@ -1169,7 +1213,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
       <c r="A51" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>200059</v>
@@ -1180,7 +1224,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="A52" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>200060</v>
@@ -1191,7 +1235,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>200061</v>
@@ -1202,7 +1246,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>200062</v>
@@ -1213,7 +1257,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>200063</v>
@@ -1224,7 +1268,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>200064</v>
@@ -1235,7 +1279,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="A57" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>200065</v>
@@ -1246,7 +1290,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
       <c r="A58" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>200066</v>
@@ -1257,7 +1301,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="A59" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>200067</v>
@@ -1268,7 +1312,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="A60" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>200068</v>
@@ -1279,7 +1323,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>200069</v>
@@ -1290,7 +1334,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
       <c r="A62" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>200070</v>
@@ -1301,7 +1345,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
       <c r="A63" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>200071</v>
@@ -1312,7 +1356,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
       <c r="A64" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>200072</v>
@@ -1323,7 +1367,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
       <c r="A65" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>200073</v>
@@ -1334,7 +1378,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
       <c r="A66" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>200074</v>
@@ -1345,7 +1389,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
       <c r="A67" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>200075</v>
@@ -1356,7 +1400,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="A68" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>200076</v>
@@ -1367,7 +1411,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
       <c r="A69" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>200077</v>
@@ -1378,7 +1422,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
       <c r="A70" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>200078</v>
@@ -1389,7 +1433,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
       <c r="A71" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>200079</v>
@@ -1400,7 +1444,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
       <c r="A72" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>200080</v>
@@ -1411,7 +1455,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
       <c r="A73" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E73" s="0" t="n">
         <v>200081</v>
@@ -1422,7 +1466,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74">
       <c r="A74" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>200082</v>
@@ -1433,7 +1477,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75">
       <c r="A75" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>200083</v>
@@ -1444,7 +1488,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
       <c r="A76" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>200084</v>
@@ -1455,7 +1499,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="77">
       <c r="A77" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>200085</v>
@@ -1466,7 +1510,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="78">
       <c r="A78" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>200086</v>
@@ -1477,7 +1521,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="79">
       <c r="A79" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>200087</v>
@@ -1488,7 +1532,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="80">
       <c r="A80" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>200088</v>
@@ -1499,7 +1543,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="81">
       <c r="A81" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>200089</v>
@@ -1510,7 +1554,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="82">
       <c r="A82" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>200090</v>
@@ -1521,7 +1565,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
       <c r="A83" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E83" s="0" t="n">
         <v>200091</v>
@@ -1532,7 +1576,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84">
       <c r="A84" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E84" s="0" t="n">
         <v>200092</v>
@@ -1543,7 +1587,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
       <c r="A85" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>200093</v>
@@ -1554,7 +1598,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
       <c r="A86" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>200094</v>
@@ -1565,7 +1609,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
       <c r="A87" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>200095</v>
@@ -1576,7 +1620,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88">
       <c r="A88" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>200096</v>
@@ -1587,7 +1631,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
       <c r="A89" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E89" s="0" t="n">
         <v>200097</v>
@@ -1598,7 +1642,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="90">
       <c r="A90" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>200098</v>
@@ -1609,7 +1653,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="91">
       <c r="A91" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E91" s="0" t="n">
         <v>200099</v>
@@ -1620,7 +1664,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
       <c r="A92" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>200100</v>
@@ -1631,7 +1675,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
       <c r="A93" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E93" s="0" t="n">
         <v>200101</v>
@@ -1642,7 +1686,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
       <c r="A94" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>200102</v>
@@ -1653,7 +1697,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95">
       <c r="A95" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>200103</v>
@@ -1664,7 +1708,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96">
       <c r="A96" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>200104</v>
@@ -1675,7 +1719,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="97">
       <c r="A97" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>200105</v>
@@ -1686,7 +1730,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="98">
       <c r="A98" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E98" s="0" t="n">
         <v>200106</v>
@@ -1697,7 +1741,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="99">
       <c r="A99" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E99" s="0" t="n">
         <v>200107</v>
@@ -1708,7 +1752,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
       <c r="A100" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>200108</v>
@@ -1719,7 +1763,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="101">
       <c r="A101" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E101" s="0" t="n">
         <v>200109</v>
@@ -1730,7 +1774,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="102">
       <c r="A102" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E102" s="0" t="n">
         <v>200110</v>
@@ -1741,7 +1785,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="103">
       <c r="A103" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E103" s="0" t="n">
         <v>200111</v>
@@ -1752,7 +1796,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="104">
       <c r="A104" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E104" s="0" t="n">
         <v>200112</v>
@@ -1763,7 +1807,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="105">
       <c r="A105" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E105" s="0" t="n">
         <v>200113</v>
@@ -1774,7 +1818,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="106">
       <c r="A106" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E106" s="0" t="n">
         <v>200114</v>
@@ -1785,7 +1829,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="107">
       <c r="A107" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E107" s="0" t="n">
         <v>200115</v>
@@ -1796,7 +1840,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="108">
       <c r="A108" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E108" s="0" t="n">
         <v>200116</v>
@@ -1807,7 +1851,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="109">
       <c r="A109" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E109" s="0" t="n">
         <v>200117</v>
@@ -1818,7 +1862,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="110">
       <c r="A110" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E110" s="0" t="n">
         <v>200118</v>
@@ -1829,7 +1873,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="111">
       <c r="A111" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E111" s="0" t="n">
         <v>200119</v>
@@ -1840,7 +1884,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="112">
       <c r="A112" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E112" s="0" t="n">
         <v>200120</v>
@@ -1851,7 +1895,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="113">
       <c r="A113" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E113" s="0" t="n">
         <v>200121</v>
@@ -1862,7 +1906,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="114">
       <c r="A114" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E114" s="0" t="n">
         <v>200122</v>
@@ -1873,7 +1917,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="115">
       <c r="A115" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E115" s="0" t="n">
         <v>200123</v>
@@ -1884,7 +1928,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="116">
       <c r="A116" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E116" s="0" t="n">
         <v>200124</v>
@@ -1895,7 +1939,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="117">
       <c r="A117" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E117" s="0" t="n">
         <v>200125</v>
@@ -1906,7 +1950,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="118">
       <c r="A118" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E118" s="0" t="n">
         <v>200126</v>
@@ -1917,7 +1961,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="119">
       <c r="A119" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E119" s="0" t="n">
         <v>200127</v>
@@ -1928,7 +1972,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="120">
       <c r="A120" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E120" s="0" t="n">
         <v>200128</v>
@@ -1939,7 +1983,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="121">
       <c r="A121" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E121" s="0" t="n">
         <v>200129</v>
@@ -1950,7 +1994,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="122">
       <c r="A122" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E122" s="0" t="n">
         <v>200130</v>
@@ -1961,7 +2005,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="123">
       <c r="A123" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E123" s="0" t="n">
         <v>200131</v>
@@ -1972,7 +2016,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="124">
       <c r="A124" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E124" s="0" t="n">
         <v>200132</v>
@@ -1983,7 +2027,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="125">
       <c r="A125" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E125" s="0" t="n">
         <v>200133</v>
@@ -1994,7 +2038,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="126">
       <c r="A126" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E126" s="0" t="n">
         <v>200134</v>
@@ -2005,7 +2049,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="127">
       <c r="A127" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E127" s="0" t="n">
         <v>200135</v>
@@ -2016,7 +2060,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="128">
       <c r="A128" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E128" s="0" t="n">
         <v>200136</v>
@@ -2027,7 +2071,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="129">
       <c r="A129" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E129" s="0" t="n">
         <v>200137</v>
@@ -2038,7 +2082,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="130">
       <c r="A130" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E130" s="0" t="n">
         <v>200138</v>
@@ -2049,7 +2093,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="131">
       <c r="A131" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E131" s="0" t="n">
         <v>200139</v>
@@ -2060,7 +2104,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="132">
       <c r="A132" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E132" s="0" t="n">
         <v>200140</v>
@@ -2071,7 +2115,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="133">
       <c r="A133" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E133" s="0" t="n">
         <v>200141</v>
@@ -2082,7 +2126,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="134">
       <c r="A134" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E134" s="0" t="n">
         <v>200142</v>
@@ -2093,7 +2137,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="135">
       <c r="A135" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E135" s="0" t="n">
         <v>200143</v>
@@ -2104,7 +2148,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="136">
       <c r="A136" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E136" s="0" t="n">
         <v>200144</v>
@@ -2115,7 +2159,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="137">
       <c r="A137" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E137" s="0" t="n">
         <v>200145</v>
@@ -2126,7 +2170,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="138">
       <c r="A138" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E138" s="0" t="n">
         <v>200146</v>
@@ -2137,7 +2181,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="139">
       <c r="A139" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E139" s="0" t="n">
         <v>200147</v>
@@ -2148,7 +2192,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="140">
       <c r="A140" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E140" s="0" t="n">
         <v>200148</v>
@@ -2159,7 +2203,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="141">
       <c r="A141" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E141" s="0" t="n">
         <v>200149</v>
@@ -2170,7 +2214,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="142">
       <c r="A142" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E142" s="0" t="n">
         <v>200150</v>
@@ -2181,7 +2225,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="143">
       <c r="A143" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E143" s="0" t="n">
         <v>200151</v>
@@ -2192,7 +2236,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="144">
       <c r="A144" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E144" s="0" t="n">
         <v>200152</v>
@@ -2203,7 +2247,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="145">
       <c r="A145" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E145" s="0" t="n">
         <v>200153</v>
@@ -2214,7 +2258,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="146">
       <c r="A146" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E146" s="0" t="n">
         <v>200154</v>
@@ -2225,7 +2269,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="147">
       <c r="A147" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E147" s="0" t="n">
         <v>200155</v>
@@ -2236,7 +2280,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="148">
       <c r="A148" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E148" s="0" t="n">
         <v>200156</v>
@@ -2247,7 +2291,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="149">
       <c r="A149" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E149" s="0" t="n">
         <v>200157</v>
@@ -2258,7 +2302,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="150">
       <c r="A150" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E150" s="0" t="n">
         <v>200158</v>
@@ -2269,7 +2313,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="151">
       <c r="A151" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E151" s="0" t="n">
         <v>200159</v>
@@ -2280,7 +2324,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="152">
       <c r="A152" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E152" s="0" t="n">
         <v>200160</v>
@@ -2291,7 +2335,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="153">
       <c r="A153" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E153" s="0" t="n">
         <v>200161</v>
@@ -2302,7 +2346,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="154">
       <c r="A154" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E154" s="0" t="n">
         <v>200162</v>
@@ -2313,7 +2357,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="155">
       <c r="A155" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E155" s="0" t="n">
         <v>200163</v>
@@ -2324,7 +2368,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="156">
       <c r="A156" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E156" s="0" t="n">
         <v>200164</v>
@@ -2335,7 +2379,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="157">
       <c r="A157" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E157" s="0" t="n">
         <v>200165</v>
@@ -2346,7 +2390,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="158">
       <c r="A158" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E158" s="0" t="n">
         <v>200166</v>
@@ -2357,7 +2401,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="159">
       <c r="A159" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E159" s="0" t="n">
         <v>200167</v>
@@ -2368,7 +2412,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="160">
       <c r="A160" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E160" s="0" t="n">
         <v>200168</v>
@@ -2379,7 +2423,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="161">
       <c r="A161" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E161" s="0" t="n">
         <v>200169</v>
@@ -2390,7 +2434,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="162">
       <c r="A162" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E162" s="0" t="n">
         <v>200170</v>
@@ -2401,7 +2445,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="163">
       <c r="A163" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E163" s="0" t="n">
         <v>200171</v>
@@ -2412,7 +2456,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="164">
       <c r="A164" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E164" s="0" t="n">
         <v>200172</v>
@@ -2423,7 +2467,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="165">
       <c r="A165" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E165" s="0" t="n">
         <v>200173</v>
@@ -2434,7 +2478,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="166">
       <c r="A166" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E166" s="0" t="n">
         <v>200174</v>
@@ -2445,7 +2489,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="167">
       <c r="A167" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E167" s="0" t="n">
         <v>200175</v>
@@ -2456,7 +2500,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="168">
       <c r="A168" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E168" s="0" t="n">
         <v>200176</v>
@@ -2467,7 +2511,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="169">
       <c r="A169" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E169" s="0" t="n">
         <v>200177</v>
@@ -2478,7 +2522,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="170">
       <c r="A170" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E170" s="0" t="n">
         <v>200178</v>
@@ -2489,7 +2533,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="171">
       <c r="A171" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E171" s="0" t="n">
         <v>200179</v>
@@ -2500,7 +2544,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="172">
       <c r="A172" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E172" s="0" t="n">
         <v>200180</v>
@@ -2511,7 +2555,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="173">
       <c r="A173" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E173" s="0" t="n">
         <v>200181</v>
@@ -2522,7 +2566,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="174">
       <c r="A174" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E174" s="0" t="n">
         <v>200182</v>
@@ -2533,7 +2577,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="175">
       <c r="A175" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E175" s="0" t="n">
         <v>200183</v>
@@ -2544,7 +2588,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="176">
       <c r="A176" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E176" s="0" t="n">
         <v>200184</v>
@@ -2555,7 +2599,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="177">
       <c r="A177" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E177" s="0" t="n">
         <v>200185</v>
@@ -2566,7 +2610,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="178">
       <c r="A178" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E178" s="0" t="n">
         <v>200186</v>
@@ -2577,7 +2621,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="179">
       <c r="A179" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E179" s="0" t="n">
         <v>200187</v>
@@ -2588,7 +2632,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="180">
       <c r="A180" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E180" s="0" t="n">
         <v>200188</v>
@@ -2599,7 +2643,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="181">
       <c r="A181" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E181" s="0" t="n">
         <v>200189</v>
@@ -2610,7 +2654,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="182">
       <c r="A182" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E182" s="0" t="n">
         <v>200190</v>
@@ -2621,7 +2665,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="183">
       <c r="A183" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E183" s="0" t="n">
         <v>200191</v>
@@ -2632,7 +2676,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="184">
       <c r="A184" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E184" s="0" t="n">
         <v>200192</v>
@@ -2643,7 +2687,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="185">
       <c r="A185" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E185" s="0" t="n">
         <v>200193</v>
@@ -2654,7 +2698,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="186">
       <c r="A186" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E186" s="0" t="n">
         <v>200194</v>
@@ -2665,7 +2709,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="187">
       <c r="A187" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E187" s="0" t="n">
         <v>200195</v>
@@ -2676,7 +2720,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="188">
       <c r="A188" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E188" s="0" t="n">
         <v>200196</v>
@@ -2687,7 +2731,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="189">
       <c r="A189" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E189" s="0" t="n">
         <v>200197</v>
@@ -2698,7 +2742,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="190">
       <c r="A190" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E190" s="0" t="n">
         <v>200198</v>
@@ -2709,7 +2753,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="191">
       <c r="A191" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E191" s="0" t="n">
         <v>200199</v>
@@ -2720,7 +2764,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="192">
       <c r="A192" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E192" s="0" t="n">
         <v>200200</v>
@@ -2731,7 +2775,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="193">
       <c r="A193" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E193" s="0" t="n">
         <v>200201</v>
@@ -2742,7 +2786,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="194">
       <c r="A194" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E194" s="0" t="n">
         <v>200202</v>
@@ -2753,7 +2797,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="195">
       <c r="A195" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E195" s="0" t="n">
         <v>200203</v>
@@ -2764,7 +2808,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="196">
       <c r="A196" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E196" s="0" t="n">
         <v>200204</v>
@@ -2775,7 +2819,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="197">
       <c r="A197" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E197" s="0" t="n">
         <v>200207</v>
@@ -2786,7 +2830,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="198">
       <c r="A198" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E198" s="0" t="n">
         <v>200209</v>
@@ -2797,7 +2841,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="199">
       <c r="A199" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E199" s="0" t="n">
         <v>200211</v>
@@ -2808,7 +2852,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="200">
       <c r="A200" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E200" s="0" t="n">
         <v>200212</v>
@@ -2819,7 +2863,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="201">
       <c r="A201" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E201" s="0" t="n">
         <v>200213</v>
@@ -2830,7 +2874,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="202">
       <c r="A202" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E202" s="0" t="n">
         <v>200214</v>
@@ -2841,7 +2885,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="203">
       <c r="A203" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E203" s="0" t="n">
         <v>200215</v>
@@ -2852,7 +2896,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="204">
       <c r="A204" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E204" s="0" t="n">
         <v>200216</v>
@@ -2863,7 +2907,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="205">
       <c r="A205" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E205" s="0" t="n">
         <v>200217</v>
@@ -2874,7 +2918,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="206">
       <c r="A206" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E206" s="0" t="n">
         <v>200218</v>
@@ -2885,7 +2929,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="207">
       <c r="A207" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E207" s="0" t="n">
         <v>200219</v>
@@ -2896,7 +2940,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="208">
       <c r="A208" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E208" s="0" t="n">
         <v>200220</v>
@@ -2907,7 +2951,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="209">
       <c r="A209" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E209" s="0" t="n">
         <v>200221</v>
@@ -2918,7 +2962,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="210">
       <c r="A210" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E210" s="0" t="n">
         <v>200222</v>
@@ -2929,7 +2973,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="211">
       <c r="A211" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E211" s="0" t="n">
         <v>200223</v>
@@ -2940,7 +2984,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="212">
       <c r="A212" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E212" s="0" t="n">
         <v>200224</v>
@@ -2951,7 +2995,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="213">
       <c r="A213" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E213" s="0" t="n">
         <v>200225</v>
@@ -2962,7 +3006,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="214">
       <c r="A214" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E214" s="0" t="n">
         <v>200226</v>
@@ -2973,7 +3017,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="215">
       <c r="A215" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E215" s="0" t="n">
         <v>200227</v>
@@ -2984,7 +3028,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="216">
       <c r="A216" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E216" s="0" t="n">
         <v>200228</v>
@@ -2995,7 +3039,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="217">
       <c r="A217" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E217" s="0" t="n">
         <v>200229</v>
@@ -3006,7 +3050,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="218">
       <c r="A218" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E218" s="0" t="n">
         <v>200230</v>
@@ -3017,7 +3061,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="219">
       <c r="A219" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E219" s="0" t="n">
         <v>200231</v>
@@ -3028,7 +3072,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="220">
       <c r="A220" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E220" s="0" t="n">
         <v>200232</v>
@@ -3039,7 +3083,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="221">
       <c r="A221" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E221" s="0" t="n">
         <v>200233</v>
@@ -3050,7 +3094,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="222">
       <c r="A222" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E222" s="0" t="n">
         <v>200234</v>
@@ -3061,7 +3105,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="223">
       <c r="A223" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E223" s="0" t="n">
         <v>200235</v>
@@ -3072,7 +3116,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="224">
       <c r="A224" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E224" s="0" t="n">
         <v>200236</v>
@@ -3083,7 +3127,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="225">
       <c r="A225" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E225" s="0" t="n">
         <v>200237</v>
@@ -3094,7 +3138,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="226">
       <c r="A226" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E226" s="0" t="n">
         <v>200238</v>
@@ -3105,7 +3149,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="227">
       <c r="A227" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E227" s="0" t="n">
         <v>200239</v>
@@ -3116,7 +3160,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="228">
       <c r="A228" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E228" s="0" t="n">
         <v>200240</v>
@@ -3127,7 +3171,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="229">
       <c r="A229" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E229" s="0" t="n">
         <v>200241</v>
@@ -3138,7 +3182,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="230">
       <c r="A230" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E230" s="0" t="n">
         <v>200242</v>
@@ -3149,7 +3193,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="231">
       <c r="A231" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E231" s="0" t="n">
         <v>200243</v>
@@ -3160,7 +3204,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="232">
       <c r="A232" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E232" s="0" t="n">
         <v>200244</v>
@@ -3171,7 +3215,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="233">
       <c r="A233" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E233" s="0" t="n">
         <v>200245</v>
@@ -3182,7 +3226,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="234">
       <c r="A234" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E234" s="0" t="n">
         <v>200246</v>
@@ -3193,7 +3237,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="235">
       <c r="A235" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E235" s="0" t="n">
         <v>200247</v>
@@ -3204,7 +3248,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="236">
       <c r="A236" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E236" s="0" t="n">
         <v>200248</v>
@@ -3215,7 +3259,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="237">
       <c r="A237" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E237" s="0" t="n">
         <v>200249</v>
@@ -3226,7 +3270,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="238">
       <c r="A238" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E238" s="0" t="n">
         <v>200250</v>
@@ -3237,7 +3281,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="239">
       <c r="A239" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E239" s="0" t="n">
         <v>200251</v>
@@ -3248,7 +3292,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="240">
       <c r="A240" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E240" s="0" t="n">
         <v>200252</v>
@@ -3259,7 +3303,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="241">
       <c r="A241" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E241" s="0" t="n">
         <v>200253</v>
@@ -3270,7 +3314,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="242">
       <c r="A242" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E242" s="0" t="n">
         <v>200254</v>
@@ -3281,7 +3325,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="243">
       <c r="A243" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E243" s="0" t="n">
         <v>200255</v>
@@ -3292,7 +3336,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="244">
       <c r="A244" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E244" s="0" t="n">
         <v>200256</v>
@@ -3303,7 +3347,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="245">
       <c r="A245" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E245" s="0" t="n">
         <v>200257</v>
@@ -3314,7 +3358,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="246">
       <c r="A246" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E246" s="0" t="n">
         <v>200258</v>
@@ -3325,7 +3369,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="247">
       <c r="A247" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E247" s="0" t="n">
         <v>200259</v>
@@ -3336,7 +3380,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="248">
       <c r="A248" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E248" s="0" t="n">
         <v>200260</v>
@@ -3347,7 +3391,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="249">
       <c r="A249" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E249" s="0" t="n">
         <v>200261</v>
@@ -3358,7 +3402,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="250">
       <c r="A250" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E250" s="0" t="n">
         <v>200262</v>
@@ -3369,7 +3413,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="251">
       <c r="A251" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E251" s="0" t="n">
         <v>200263</v>
@@ -3380,7 +3424,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="252">
       <c r="A252" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E252" s="0" t="n">
         <v>200264</v>
@@ -3391,7 +3435,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="253">
       <c r="A253" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E253" s="0" t="n">
         <v>200265</v>
@@ -3402,7 +3446,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="254">
       <c r="A254" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E254" s="0" t="n">
         <v>200266</v>
@@ -3413,7 +3457,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="255">
       <c r="A255" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E255" s="0" t="n">
         <v>200267</v>
@@ -3424,7 +3468,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="256">
       <c r="A256" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E256" s="0" t="n">
         <v>200268</v>
@@ -3435,7 +3479,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="257">
       <c r="A257" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E257" s="0" t="n">
         <v>200269</v>
@@ -3446,7 +3490,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="258">
       <c r="A258" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E258" s="0" t="n">
         <v>200270</v>
@@ -3457,7 +3501,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="259">
       <c r="A259" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E259" s="0" t="n">
         <v>200271</v>
@@ -3468,7 +3512,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="260">
       <c r="A260" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E260" s="0" t="n">
         <v>200272</v>
@@ -3479,7 +3523,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="261">
       <c r="A261" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E261" s="0" t="n">
         <v>200273</v>
@@ -3490,7 +3534,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="262">
       <c r="A262" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E262" s="0" t="n">
         <v>200274</v>
@@ -3501,7 +3545,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="263">
       <c r="A263" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E263" s="0" t="n">
         <v>200275</v>
@@ -3512,7 +3556,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="264">
       <c r="A264" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E264" s="0" t="n">
         <v>200276</v>
@@ -3523,7 +3567,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="265">
       <c r="A265" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E265" s="0" t="n">
         <v>200277</v>
@@ -3534,7 +3578,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="266">
       <c r="A266" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E266" s="0" t="n">
         <v>200278</v>
@@ -3545,7 +3589,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="267">
       <c r="A267" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E267" s="0" t="n">
         <v>200279</v>
@@ -3556,7 +3600,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="268">
       <c r="A268" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E268" s="0" t="n">
         <v>200280</v>
@@ -3567,7 +3611,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="269">
       <c r="A269" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E269" s="0" t="n">
         <v>200281</v>
@@ -3578,7 +3622,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="270">
       <c r="A270" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E270" s="0" t="n">
         <v>200282</v>
@@ -3589,7 +3633,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="271">
       <c r="A271" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E271" s="0" t="n">
         <v>200283</v>
@@ -3600,7 +3644,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="272">
       <c r="A272" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E272" s="0" t="n">
         <v>200284</v>
@@ -3611,7 +3655,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="273">
       <c r="A273" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E273" s="0" t="n">
         <v>200285</v>
@@ -3622,7 +3666,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="274">
       <c r="A274" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E274" s="0" t="n">
         <v>200286</v>
@@ -3633,7 +3677,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="275">
       <c r="A275" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E275" s="0" t="n">
         <v>200287</v>
@@ -3644,7 +3688,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="276">
       <c r="A276" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E276" s="0" t="n">
         <v>200288</v>
@@ -3655,7 +3699,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="277">
       <c r="A277" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E277" s="0" t="n">
         <v>200289</v>
@@ -3666,7 +3710,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="278">
       <c r="A278" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E278" s="0" t="n">
         <v>200290</v>
@@ -3677,7 +3721,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="279">
       <c r="A279" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E279" s="0" t="n">
         <v>200291</v>
@@ -3688,7 +3732,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="280">
       <c r="A280" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E280" s="0" t="n">
         <v>200292</v>
@@ -3699,7 +3743,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="281">
       <c r="A281" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E281" s="0" t="n">
         <v>200293</v>
@@ -3710,7 +3754,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="282">
       <c r="A282" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E282" s="0" t="n">
         <v>200294</v>
@@ -3721,7 +3765,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="283">
       <c r="A283" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E283" s="0" t="n">
         <v>200295</v>
@@ -3732,7 +3776,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="284">
       <c r="A284" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E284" s="0" t="n">
         <v>200296</v>
@@ -3743,7 +3787,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="285">
       <c r="A285" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E285" s="0" t="n">
         <v>200297</v>
@@ -3754,7 +3798,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="286">
       <c r="A286" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E286" s="0" t="n">
         <v>200298</v>
@@ -3765,7 +3809,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="287">
       <c r="A287" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E287" s="0" t="n">
         <v>200299</v>
@@ -3776,7 +3820,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="288">
       <c r="A288" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E288" s="0" t="n">
         <v>200300</v>
@@ -3787,7 +3831,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="289">
       <c r="A289" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E289" s="0" t="n">
         <v>200301</v>
@@ -3798,7 +3842,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="290">
       <c r="A290" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E290" s="0" t="n">
         <v>200302</v>
@@ -3809,7 +3853,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="291">
       <c r="A291" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E291" s="0" t="n">
         <v>200303</v>
@@ -3820,7 +3864,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="292">
       <c r="A292" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E292" s="0" t="n">
         <v>200304</v>
@@ -3831,7 +3875,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="293">
       <c r="A293" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E293" s="0" t="n">
         <v>200305</v>
@@ -3842,7 +3886,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="294">
       <c r="A294" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E294" s="0" t="n">
         <v>200306</v>
@@ -3853,7 +3897,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="295">
       <c r="A295" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E295" s="0" t="n">
         <v>200307</v>
@@ -3864,7 +3908,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="296">
       <c r="A296" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E296" s="0" t="n">
         <v>200309</v>
@@ -3875,7 +3919,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="297">
       <c r="A297" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E297" s="0" t="n">
         <v>200310</v>
@@ -3886,7 +3930,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="298">
       <c r="A298" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E298" s="0" t="n">
         <v>200311</v>
@@ -3897,7 +3941,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="299">
       <c r="A299" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E299" s="0" t="n">
         <v>200312</v>
@@ -3908,7 +3952,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="300">
       <c r="A300" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E300" s="0" t="n">
         <v>200313</v>
@@ -3919,7 +3963,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="301">
       <c r="A301" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E301" s="0" t="n">
         <v>200314</v>
@@ -3930,7 +3974,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="302">
       <c r="A302" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E302" s="0" t="n">
         <v>200315</v>
@@ -3941,7 +3985,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="303">
       <c r="A303" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E303" s="0" t="n">
         <v>200316</v>
@@ -3952,7 +3996,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="304">
       <c r="A304" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E304" s="0" t="n">
         <v>200317</v>
@@ -3963,7 +4007,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="305">
       <c r="A305" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E305" s="0" t="n">
         <v>200318</v>
@@ -3974,7 +4018,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="306">
       <c r="A306" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E306" s="0" t="n">
         <v>200319</v>
@@ -3985,7 +4029,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="307">
       <c r="A307" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E307" s="0" t="n">
         <v>200320</v>
@@ -3996,7 +4040,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="308">
       <c r="A308" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E308" s="0" t="n">
         <v>200321</v>
@@ -4007,7 +4051,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="309">
       <c r="A309" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E309" s="0" t="n">
         <v>200322</v>
@@ -4018,7 +4062,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="310">
       <c r="A310" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E310" s="0" t="n">
         <v>200323</v>
@@ -4029,7 +4073,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="311">
       <c r="A311" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E311" s="0" t="n">
         <v>200324</v>
@@ -4040,7 +4084,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="312">
       <c r="A312" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E312" s="0" t="n">
         <v>200325</v>
@@ -4051,7 +4095,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="313">
       <c r="A313" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E313" s="0" t="n">
         <v>200326</v>
@@ -4062,7 +4106,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="314">
       <c r="A314" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E314" s="0" t="n">
         <v>200327</v>
@@ -4073,7 +4117,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="315">
       <c r="A315" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E315" s="0" t="n">
         <v>200328</v>
@@ -4084,7 +4128,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="316">
       <c r="A316" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E316" s="0" t="n">
         <v>200329</v>
@@ -4095,7 +4139,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="317">
       <c r="A317" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E317" s="0" t="n">
         <v>200330</v>
@@ -4106,7 +4150,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="318">
       <c r="A318" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E318" s="0" t="n">
         <v>200331</v>
@@ -4117,7 +4161,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="319">
       <c r="A319" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E319" s="0" t="n">
         <v>200332</v>
@@ -4128,7 +4172,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="320">
       <c r="A320" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E320" s="0" t="n">
         <v>200333</v>
@@ -4139,7 +4183,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="321">
       <c r="A321" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E321" s="0" t="n">
         <v>200334</v>
@@ -4150,7 +4194,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="322">
       <c r="A322" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E322" s="0" t="n">
         <v>200335</v>
@@ -4161,7 +4205,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="323">
       <c r="A323" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E323" s="0" t="n">
         <v>200336</v>
@@ -4172,7 +4216,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="324">
       <c r="A324" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E324" s="0" t="n">
         <v>200337</v>
@@ -4183,7 +4227,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="325">
       <c r="A325" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E325" s="0" t="n">
         <v>200338</v>
@@ -4194,7 +4238,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="326">
       <c r="A326" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E326" s="0" t="n">
         <v>200339</v>
@@ -4205,7 +4249,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="327">
       <c r="A327" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E327" s="0" t="n">
         <v>200340</v>
@@ -4216,7 +4260,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="328">
       <c r="A328" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E328" s="0" t="n">
         <v>200341</v>
@@ -4227,7 +4271,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="329">
       <c r="A329" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E329" s="0" t="n">
         <v>200342</v>
@@ -4238,7 +4282,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="330">
       <c r="A330" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E330" s="0" t="n">
         <v>200343</v>
@@ -4249,7 +4293,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="331">
       <c r="A331" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E331" s="0" t="n">
         <v>200344</v>
@@ -4260,7 +4304,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="332">
       <c r="A332" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E332" s="0" t="n">
         <v>200345</v>
@@ -4271,7 +4315,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="333">
       <c r="A333" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E333" s="0" t="n">
         <v>200346</v>
@@ -4282,7 +4326,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="334">
       <c r="A334" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E334" s="0" t="n">
         <v>200347</v>
@@ -4293,7 +4337,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="335">
       <c r="A335" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E335" s="0" t="n">
         <v>200348</v>
@@ -4304,7 +4348,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="336">
       <c r="A336" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E336" s="0" t="n">
         <v>200349</v>
@@ -4315,7 +4359,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="337">
       <c r="A337" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E337" s="0" t="n">
         <v>200350</v>
@@ -4326,7 +4370,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="338">
       <c r="A338" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E338" s="0" t="n">
         <v>200351</v>
@@ -4337,7 +4381,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="339">
       <c r="A339" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E339" s="0" t="n">
         <v>200352</v>
@@ -4348,7 +4392,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="340">
       <c r="A340" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E340" s="0" t="n">
         <v>200353</v>
@@ -4359,7 +4403,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="341">
       <c r="A341" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E341" s="0" t="n">
         <v>200354</v>
@@ -4370,7 +4414,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="342">
       <c r="A342" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E342" s="0" t="n">
         <v>200355</v>
@@ -4381,7 +4425,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="343">
       <c r="A343" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E343" s="0" t="n">
         <v>200356</v>
@@ -4392,7 +4436,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="344">
       <c r="A344" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E344" s="0" t="n">
         <v>200357</v>
@@ -4403,7 +4447,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="345">
       <c r="A345" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E345" s="0" t="n">
         <v>200358</v>
@@ -4414,7 +4458,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="346">
       <c r="A346" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E346" s="0" t="n">
         <v>200359</v>
@@ -4425,7 +4469,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="347">
       <c r="A347" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E347" s="0" t="n">
         <v>200360</v>
@@ -4436,7 +4480,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="348">
       <c r="A348" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E348" s="0" t="n">
         <v>200361</v>
@@ -4447,7 +4491,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="349">
       <c r="A349" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E349" s="0" t="n">
         <v>200362</v>
@@ -4458,7 +4502,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="350">
       <c r="A350" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E350" s="0" t="n">
         <v>200363</v>
@@ -4469,7 +4513,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="351">
       <c r="A351" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E351" s="0" t="n">
         <v>200364</v>
@@ -4480,7 +4524,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="352">
       <c r="A352" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E352" s="0" t="n">
         <v>200365</v>
@@ -4491,7 +4535,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="353">
       <c r="A353" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E353" s="0" t="n">
         <v>200366</v>
@@ -4502,7 +4546,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="354">
       <c r="A354" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E354" s="0" t="n">
         <v>200367</v>
@@ -4513,7 +4557,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="355">
       <c r="A355" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E355" s="0" t="n">
         <v>200368</v>
@@ -4524,7 +4568,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="356">
       <c r="A356" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E356" s="0" t="n">
         <v>200369</v>
@@ -4535,7 +4579,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="357">
       <c r="A357" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E357" s="0" t="n">
         <v>200370</v>
@@ -4546,7 +4590,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="358">
       <c r="A358" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E358" s="0" t="n">
         <v>200371</v>
@@ -4557,7 +4601,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="359">
       <c r="A359" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E359" s="0" t="n">
         <v>200372</v>
@@ -4568,7 +4612,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="360">
       <c r="A360" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E360" s="0" t="n">
         <v>200373</v>
@@ -4579,7 +4623,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="361">
       <c r="A361" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E361" s="0" t="n">
         <v>200374</v>
@@ -4590,7 +4634,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="362">
       <c r="A362" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E362" s="0" t="n">
         <v>200375</v>
@@ -4601,7 +4645,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="363">
       <c r="A363" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E363" s="0" t="n">
         <v>200376</v>
@@ -4612,7 +4656,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="364">
       <c r="A364" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E364" s="0" t="n">
         <v>200377</v>
@@ -4623,7 +4667,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="365">
       <c r="A365" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E365" s="0" t="n">
         <v>200378</v>
@@ -4634,7 +4678,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="366">
       <c r="A366" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E366" s="0" t="n">
         <v>200379</v>
@@ -4645,7 +4689,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="367">
       <c r="A367" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E367" s="0" t="n">
         <v>200380</v>
@@ -4656,7 +4700,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="368">
       <c r="A368" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E368" s="0" t="n">
         <v>200381</v>
@@ -4667,7 +4711,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="369">
       <c r="A369" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E369" s="0" t="n">
         <v>200382</v>
@@ -4678,7 +4722,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="370">
       <c r="A370" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E370" s="0" t="n">
         <v>200383</v>
@@ -4689,7 +4733,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="371">
       <c r="A371" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E371" s="0" t="n">
         <v>200390</v>
@@ -4700,7 +4744,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="372">
       <c r="A372" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E372" s="0" t="n">
         <v>200392</v>
@@ -4711,7 +4755,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="373">
       <c r="A373" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E373" s="0" t="n">
         <v>200394</v>
@@ -4722,7 +4766,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="374">
       <c r="A374" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E374" s="0" t="n">
         <v>200396</v>
@@ -4733,7 +4777,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="375">
       <c r="A375" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E375" s="0" t="n">
         <v>200399</v>
@@ -4744,7 +4788,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="376">
       <c r="A376" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E376" s="0" t="n">
         <v>200400</v>
@@ -4755,7 +4799,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="377">
       <c r="A377" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E377" s="0" t="n">
         <v>200401</v>
@@ -4766,7 +4810,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="378">
       <c r="A378" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E378" s="0" t="n">
         <v>200402</v>
@@ -4777,7 +4821,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="379">
       <c r="A379" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E379" s="0" t="n">
         <v>200403</v>
@@ -4788,7 +4832,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="380">
       <c r="A380" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E380" s="0" t="n">
         <v>200404</v>
@@ -4799,7 +4843,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="381">
       <c r="A381" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E381" s="0" t="n">
         <v>200405</v>
@@ -4810,7 +4854,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="382">
       <c r="A382" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E382" s="0" t="n">
         <v>200406</v>
@@ -4821,7 +4865,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="383">
       <c r="A383" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E383" s="0" t="n">
         <v>200407</v>
@@ -4832,7 +4876,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="384">
       <c r="A384" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E384" s="0" t="n">
         <v>200408</v>
@@ -4843,7 +4887,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="385">
       <c r="A385" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E385" s="0" t="n">
         <v>200409</v>
@@ -4854,7 +4898,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="386">
       <c r="A386" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E386" s="0" t="n">
         <v>200410</v>
@@ -4865,7 +4909,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="387">
       <c r="A387" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E387" s="0" t="n">
         <v>200411</v>
@@ -4876,7 +4920,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="388">
       <c r="A388" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E388" s="0" t="n">
         <v>200412</v>
@@ -4887,7 +4931,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="389">
       <c r="A389" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E389" s="0" t="n">
         <v>200413</v>
@@ -4898,7 +4942,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="390">
       <c r="A390" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E390" s="0" t="n">
         <v>200414</v>
@@ -4909,7 +4953,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="391">
       <c r="A391" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E391" s="0" t="n">
         <v>200415</v>
@@ -4920,7 +4964,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="392">
       <c r="A392" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E392" s="0" t="n">
         <v>200416</v>
@@ -4931,7 +4975,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="393">
       <c r="A393" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E393" s="0" t="n">
         <v>200417</v>
@@ -4942,7 +4986,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="394">
       <c r="A394" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E394" s="0" t="n">
         <v>200418</v>
@@ -4953,7 +4997,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="395">
       <c r="A395" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E395" s="0" t="n">
         <v>200419</v>
@@ -4964,7 +5008,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="396">
       <c r="A396" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E396" s="0" t="n">
         <v>200420</v>
@@ -4975,7 +5019,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="397">
       <c r="A397" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E397" s="0" t="n">
         <v>200421</v>
@@ -4986,7 +5030,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="398">
       <c r="A398" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E398" s="0" t="n">
         <v>200422</v>
@@ -4997,7 +5041,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="399">
       <c r="A399" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E399" s="0" t="n">
         <v>200423</v>
@@ -5008,7 +5052,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="400">
       <c r="A400" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E400" s="0" t="n">
         <v>200424</v>
@@ -5019,7 +5063,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="401">
       <c r="A401" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E401" s="0" t="n">
         <v>200425</v>
@@ -5030,7 +5074,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="402">
       <c r="A402" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E402" s="0" t="n">
         <v>200426</v>
@@ -5041,7 +5085,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="403">
       <c r="A403" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E403" s="0" t="n">
         <v>200427</v>
@@ -5052,7 +5096,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="404">
       <c r="A404" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E404" s="0" t="n">
         <v>200428</v>
@@ -5063,7 +5107,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="405">
       <c r="A405" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E405" s="0" t="n">
         <v>200429</v>
@@ -5074,7 +5118,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="406">
       <c r="A406" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E406" s="0" t="n">
         <v>200430</v>
@@ -5085,7 +5129,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="407">
       <c r="A407" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E407" s="0" t="n">
         <v>200431</v>
@@ -5096,7 +5140,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="408">
       <c r="A408" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E408" s="0" t="n">
         <v>200432</v>
@@ -5107,7 +5151,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="409">
       <c r="A409" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E409" s="0" t="n">
         <v>200433</v>
@@ -5118,7 +5162,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="410">
       <c r="A410" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E410" s="0" t="n">
         <v>200434</v>
@@ -5129,7 +5173,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="411">
       <c r="A411" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E411" s="0" t="n">
         <v>200435</v>
@@ -5140,7 +5184,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="412">
       <c r="A412" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E412" s="0" t="n">
         <v>200436</v>
@@ -5151,7 +5195,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="413">
       <c r="A413" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E413" s="0" t="n">
         <v>200437</v>
@@ -5162,7 +5206,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="414">
       <c r="A414" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E414" s="0" t="n">
         <v>200438</v>
@@ -5173,7 +5217,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="415">
       <c r="A415" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E415" s="0" t="n">
         <v>200439</v>
@@ -5184,7 +5228,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="416">
       <c r="A416" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E416" s="0" t="n">
         <v>200440</v>
@@ -5195,7 +5239,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="417">
       <c r="A417" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E417" s="0" t="n">
         <v>200441</v>
@@ -5206,7 +5250,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="418">
       <c r="A418" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E418" s="0" t="n">
         <v>200442</v>
@@ -5217,7 +5261,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="419">
       <c r="A419" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E419" s="0" t="n">
         <v>200443</v>
@@ -5228,7 +5272,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="420">
       <c r="A420" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E420" s="0" t="n">
         <v>200444</v>
@@ -5239,7 +5283,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="421">
       <c r="A421" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E421" s="0" t="n">
         <v>200445</v>
@@ -5250,7 +5294,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="422">
       <c r="A422" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E422" s="0" t="n">
         <v>200446</v>
@@ -5261,7 +5305,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="423">
       <c r="A423" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E423" s="0" t="n">
         <v>200447</v>
@@ -5272,7 +5316,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="424">
       <c r="A424" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E424" s="0" t="n">
         <v>200448</v>
@@ -5283,7 +5327,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="425">
       <c r="A425" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E425" s="0" t="n">
         <v>200449</v>
@@ -5294,7 +5338,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="426">
       <c r="A426" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E426" s="0" t="n">
         <v>200450</v>
@@ -5305,7 +5349,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="427">
       <c r="A427" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E427" s="0" t="n">
         <v>200451</v>
@@ -5316,7 +5360,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="428">
       <c r="A428" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E428" s="0" t="n">
         <v>200454</v>
@@ -5327,7 +5371,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="429">
       <c r="A429" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E429" s="0" t="n">
         <v>200455</v>
@@ -5338,7 +5382,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="430">
       <c r="A430" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E430" s="0" t="n">
         <v>200456</v>
@@ -5349,7 +5393,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="431">
       <c r="A431" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E431" s="0" t="n">
         <v>200457</v>
@@ -5360,7 +5404,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="432">
       <c r="A432" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E432" s="0" t="n">
         <v>200458</v>
@@ -5371,7 +5415,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="433">
       <c r="A433" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E433" s="0" t="n">
         <v>200459</v>
@@ -5382,7 +5426,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="434">
       <c r="A434" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E434" s="0" t="n">
         <v>200460</v>
@@ -5393,7 +5437,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="435">
       <c r="A435" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E435" s="0" t="n">
         <v>200461</v>
@@ -5404,7 +5448,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="436">
       <c r="A436" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E436" s="0" t="n">
         <v>200462</v>
@@ -5415,7 +5459,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="437">
       <c r="A437" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E437" s="0" t="n">
         <v>200463</v>
@@ -5426,7 +5470,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="438">
       <c r="A438" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E438" s="0" t="n">
         <v>200464</v>
@@ -5437,7 +5481,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="439">
       <c r="A439" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E439" s="0" t="n">
         <v>200465</v>
@@ -5448,7 +5492,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="440">
       <c r="A440" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E440" s="0" t="n">
         <v>200466</v>
@@ -5459,7 +5503,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="441">
       <c r="A441" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E441" s="0" t="n">
         <v>200467</v>
@@ -5470,7 +5514,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="442">
       <c r="A442" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E442" s="0" t="n">
         <v>200468</v>
@@ -5481,7 +5525,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="443">
       <c r="A443" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E443" s="0" t="n">
         <v>200469</v>

</xml_diff>

<commit_message>
refactor reagent and batch entity models with "Reagent" and "ReagentBatch" base classes: - update foreign keys to point to relevant base classes - add reagent batch join tables to the Dataset model - add reagent batch foreign key to datapoint - update importers to reflect new schema - create revised dataset view methods and supporting classes - create revised dataset api endpoints - update all view methods referencing datasets from reagents - update field information for common reagent and reagent batch fields - update search code to reflect new schema - replace "dataset##" classes and methods with "dataset2##" classes and methods
</commit_message>
<xml_diff>
--- a/sampledata/Screen20020_HMSL10008_kinomescan.xlsx
+++ b/sampledata/Screen20020_HMSL10008_kinomescan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" state="visible" r:id="rId2"/>
@@ -217,31 +217,31 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="@" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -253,7 +253,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -262,67 +262,63 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+  <cellXfs count="6">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -332,26 +328,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A6" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A16" activeCellId="0" pane="topLeft" sqref="A16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.6734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="163.168367346939"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="11.6734693877551"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="163.168367346939"/>
-    <col collapsed="false" hidden="false" max="513" min="259" style="1" width="11.6734693877551"/>
-    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="163.168367346939"/>
-    <col collapsed="false" hidden="false" max="769" min="515" style="1" width="11.6734693877551"/>
-    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="163.168367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="771" style="1" width="11.6734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="163.168367346939"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="0" width="11.6734693877551"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="0" width="163.168367346939"/>
+    <col collapsed="false" hidden="false" max="513" min="259" style="0" width="11.6734693877551"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="0" width="163.168367346939"/>
+    <col collapsed="false" hidden="false" max="769" min="515" style="0" width="11.6734693877551"/>
+    <col collapsed="false" hidden="false" max="770" min="770" style="0" width="163.168367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="771" style="0" width="11.6734693877551"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -359,7 +355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -367,7 +363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -375,7 +371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -383,7 +379,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -391,7 +387,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -399,7 +395,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -407,15 +403,15 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -423,69 +419,68 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="65" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="128.75" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="128.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="54.35" outlineLevel="0" r="12">
-      <c r="A12" s="2" t="s">
+    <row r="12" customFormat="false" ht="54.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
-      <c r="A13" s="4" t="s">
+    <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="A14" s="4" t="s">
+    <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
-      <c r="A15" s="4" t="s">
+    <row r="15" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
-      <c r="A16" s="5" t="s">
+    <row r="16" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="0"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    </row>
+    <row r="17" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -493,7 +488,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="19">
+    <row r="19" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -504,7 +499,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -519,8 +514,8 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B8" activeCellId="0" pane="topLeft" sqref="B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -529,93 +524,93 @@
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.64795918367347"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="6" t="s">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>38</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
-      <c r="A3" s="6" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
-      <c r="A4" s="6" t="s">
+    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="A5" s="6" t="s">
+    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
-      <c r="A6" s="6" t="s">
+    <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="A7" s="6" t="s">
+    <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="A8" s="6" t="s">
+    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="A9" s="6" t="s">
+    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>48</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="A10" s="6" t="s">
+    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
-      <c r="A11" s="6" t="s">
+    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="A12" s="6" t="s">
+    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
-      <c r="A13" s="6" t="s">
+    <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -630,8 +625,8 @@
   </sheetPr>
   <dimension ref="A1:H443"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I1" activeCellId="0" pane="topLeft" sqref="I1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -646,7 +641,7 @@
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.64795918367347"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>53</v>
       </c>
@@ -672,7 +667,7 @@
         <v>38</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>60</v>
       </c>
@@ -683,7 +678,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>60</v>
       </c>
@@ -694,7 +689,7 @@
         <v>47</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>60</v>
       </c>
@@ -705,7 +700,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>60</v>
       </c>
@@ -716,7 +711,7 @@
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>60</v>
       </c>
@@ -727,7 +722,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>60</v>
       </c>
@@ -738,7 +733,7 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>60</v>
       </c>
@@ -749,7 +744,7 @@
         <v>1.1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>60</v>
       </c>
@@ -760,7 +755,7 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>60</v>
       </c>
@@ -771,7 +766,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>60</v>
       </c>
@@ -782,7 +777,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>60</v>
       </c>
@@ -793,7 +788,7 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>60</v>
       </c>
@@ -804,7 +799,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>60</v>
       </c>
@@ -815,7 +810,7 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row r="15" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>60</v>
       </c>
@@ -826,7 +821,7 @@
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+    <row r="16" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>60</v>
       </c>
@@ -837,7 +832,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row r="17" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>60</v>
       </c>
@@ -848,7 +843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>60</v>
       </c>
@@ -859,7 +854,7 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row r="19" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>60</v>
       </c>
@@ -870,7 +865,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row r="20" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>60</v>
       </c>
@@ -881,7 +876,7 @@
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row r="21" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>60</v>
       </c>
@@ -892,7 +887,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row r="22" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>60</v>
       </c>
@@ -903,7 +898,7 @@
         <v>75</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row r="23" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>60</v>
       </c>
@@ -914,7 +909,7 @@
         <v>77</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row r="24" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>60</v>
       </c>
@@ -925,7 +920,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row r="25" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>60</v>
       </c>
@@ -936,7 +931,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+    <row r="26" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>60</v>
       </c>
@@ -947,7 +942,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+    <row r="27" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>60</v>
       </c>
@@ -958,7 +953,7 @@
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row r="28" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>60</v>
       </c>
@@ -969,7 +964,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row r="29" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>60</v>
       </c>
@@ -980,7 +975,7 @@
         <v>69</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+    <row r="30" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>60</v>
       </c>
@@ -991,7 +986,7 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+    <row r="31" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>60</v>
       </c>
@@ -1002,7 +997,7 @@
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+    <row r="32" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>60</v>
       </c>
@@ -1013,7 +1008,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+    <row r="33" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>60</v>
       </c>
@@ -1024,7 +1019,7 @@
         <v>84</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row r="34" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>60</v>
       </c>
@@ -1035,7 +1030,7 @@
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row r="35" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>60</v>
       </c>
@@ -1046,7 +1041,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+    <row r="36" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>60</v>
       </c>
@@ -1057,7 +1052,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+    <row r="37" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>60</v>
       </c>
@@ -1068,7 +1063,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
+    <row r="38" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>60</v>
       </c>
@@ -1079,7 +1074,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
+    <row r="39" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>60</v>
       </c>
@@ -1090,7 +1085,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+    <row r="40" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>60</v>
       </c>
@@ -1101,7 +1096,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
+    <row r="41" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>60</v>
       </c>
@@ -1112,7 +1107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+    <row r="42" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>60</v>
       </c>
@@ -1123,7 +1118,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
+    <row r="43" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>60</v>
       </c>
@@ -1134,7 +1129,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
+    <row r="44" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>60</v>
       </c>
@@ -1145,7 +1140,7 @@
         <v>98</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
+    <row r="45" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>60</v>
       </c>
@@ -1156,7 +1151,7 @@
         <v>78</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
+    <row r="46" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>60</v>
       </c>
@@ -1167,7 +1162,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
+    <row r="47" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>60</v>
       </c>
@@ -1178,7 +1173,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
+    <row r="48" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>60</v>
       </c>
@@ -1189,7 +1184,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
+    <row r="49" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>60</v>
       </c>
@@ -1200,7 +1195,7 @@
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
+    <row r="50" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>60</v>
       </c>
@@ -1211,7 +1206,7 @@
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
+    <row r="51" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>60</v>
       </c>
@@ -1222,7 +1217,7 @@
         <v>83</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
+    <row r="52" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>60</v>
       </c>
@@ -1233,7 +1228,7 @@
         <v>82</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
+    <row r="53" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>60</v>
       </c>
@@ -1244,7 +1239,7 @@
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
+    <row r="54" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>60</v>
       </c>
@@ -1255,7 +1250,7 @@
         <v>99</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
+    <row r="55" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>60</v>
       </c>
@@ -1266,7 +1261,7 @@
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
+    <row r="56" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>60</v>
       </c>
@@ -1277,7 +1272,7 @@
         <v>84</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
+    <row r="57" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>60</v>
       </c>
@@ -1288,7 +1283,7 @@
         <v>95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
+    <row r="58" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>60</v>
       </c>
@@ -1299,7 +1294,7 @@
         <v>93</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
+    <row r="59" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>60</v>
       </c>
@@ -1310,7 +1305,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
+    <row r="60" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>60</v>
       </c>
@@ -1321,7 +1316,7 @@
         <v>89</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
+    <row r="61" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>60</v>
       </c>
@@ -1332,7 +1327,7 @@
         <v>72</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
+    <row r="62" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>60</v>
       </c>
@@ -1343,7 +1338,7 @@
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
+    <row r="63" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>60</v>
       </c>
@@ -1354,7 +1349,7 @@
         <v>98</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
+    <row r="64" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>60</v>
       </c>
@@ -1365,7 +1360,7 @@
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
+    <row r="65" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>60</v>
       </c>
@@ -1376,7 +1371,7 @@
         <v>86</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
+    <row r="66" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>60</v>
       </c>
@@ -1387,7 +1382,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
+    <row r="67" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>60</v>
       </c>
@@ -1398,7 +1393,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
+    <row r="68" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>60</v>
       </c>
@@ -1409,7 +1404,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
+    <row r="69" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>60</v>
       </c>
@@ -1420,7 +1415,7 @@
         <v>65</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
+    <row r="70" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>60</v>
       </c>
@@ -1431,7 +1426,7 @@
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
+    <row r="71" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>60</v>
       </c>
@@ -1442,7 +1437,7 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
+    <row r="72" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>60</v>
       </c>
@@ -1453,7 +1448,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
+    <row r="73" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>60</v>
       </c>
@@ -1464,7 +1459,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74">
+    <row r="74" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>60</v>
       </c>
@@ -1475,7 +1470,7 @@
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75">
+    <row r="75" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>60</v>
       </c>
@@ -1486,7 +1481,7 @@
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
+    <row r="76" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>60</v>
       </c>
@@ -1497,7 +1492,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="77">
+    <row r="77" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>60</v>
       </c>
@@ -1508,7 +1503,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="78">
+    <row r="78" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>60</v>
       </c>
@@ -1519,7 +1514,7 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="79">
+    <row r="79" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>60</v>
       </c>
@@ -1530,7 +1525,7 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="80">
+    <row r="80" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>60</v>
       </c>
@@ -1541,7 +1536,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="81">
+    <row r="81" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>60</v>
       </c>
@@ -1552,7 +1547,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="82">
+    <row r="82" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>60</v>
       </c>
@@ -1563,7 +1558,7 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
+    <row r="83" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>60</v>
       </c>
@@ -1574,7 +1569,7 @@
         <v>55</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84">
+    <row r="84" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>60</v>
       </c>
@@ -1585,7 +1580,7 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
+    <row r="85" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>60</v>
       </c>
@@ -1596,7 +1591,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
+    <row r="86" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>60</v>
       </c>
@@ -1607,7 +1602,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
+    <row r="87" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>60</v>
       </c>
@@ -1618,7 +1613,7 @@
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88">
+    <row r="88" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>60</v>
       </c>
@@ -1629,7 +1624,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
+    <row r="89" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>60</v>
       </c>
@@ -1640,7 +1635,7 @@
         <v>98</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="90">
+    <row r="90" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>60</v>
       </c>
@@ -1651,7 +1646,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="91">
+    <row r="91" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>60</v>
       </c>
@@ -1662,7 +1657,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
+    <row r="92" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>60</v>
       </c>
@@ -1673,7 +1668,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
+    <row r="93" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>60</v>
       </c>
@@ -1684,7 +1679,7 @@
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
+    <row r="94" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>60</v>
       </c>
@@ -1695,7 +1690,7 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95">
+    <row r="95" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>60</v>
       </c>
@@ -1706,7 +1701,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96">
+    <row r="96" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>60</v>
       </c>
@@ -1717,7 +1712,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="97">
+    <row r="97" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>60</v>
       </c>
@@ -1728,7 +1723,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="98">
+    <row r="98" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>60</v>
       </c>
@@ -1739,7 +1734,7 @@
         <v>99</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="99">
+    <row r="99" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>60</v>
       </c>
@@ -1750,7 +1745,7 @@
         <v>87</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
+    <row r="100" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>60</v>
       </c>
@@ -1761,7 +1756,7 @@
         <v>88</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="101">
+    <row r="101" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>60</v>
       </c>
@@ -1772,7 +1767,7 @@
         <v>98</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="102">
+    <row r="102" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>60</v>
       </c>
@@ -1783,7 +1778,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="103">
+    <row r="103" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>60</v>
       </c>
@@ -1794,7 +1789,7 @@
         <v>75</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="104">
+    <row r="104" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>60</v>
       </c>
@@ -1805,7 +1800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="105">
+    <row r="105" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>60</v>
       </c>
@@ -1816,7 +1811,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="106">
+    <row r="106" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>60</v>
       </c>
@@ -1827,7 +1822,7 @@
         <v>57</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="107">
+    <row r="107" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>60</v>
       </c>
@@ -1838,7 +1833,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="108">
+    <row r="108" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>60</v>
       </c>
@@ -1849,7 +1844,7 @@
         <v>89</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="109">
+    <row r="109" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>60</v>
       </c>
@@ -1860,7 +1855,7 @@
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="110">
+    <row r="110" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>60</v>
       </c>
@@ -1871,7 +1866,7 @@
         <v>59</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="111">
+    <row r="111" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>60</v>
       </c>
@@ -1882,7 +1877,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="112">
+    <row r="112" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>60</v>
       </c>
@@ -1893,7 +1888,7 @@
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="113">
+    <row r="113" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>60</v>
       </c>
@@ -1904,7 +1899,7 @@
         <v>95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="114">
+    <row r="114" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>60</v>
       </c>
@@ -1915,7 +1910,7 @@
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="115">
+    <row r="115" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>60</v>
       </c>
@@ -1926,7 +1921,7 @@
         <v>84</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="116">
+    <row r="116" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>60</v>
       </c>
@@ -1937,7 +1932,7 @@
         <v>76</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="117">
+    <row r="117" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>60</v>
       </c>
@@ -1948,7 +1943,7 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="118">
+    <row r="118" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>60</v>
       </c>
@@ -1959,7 +1954,7 @@
         <v>89</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="119">
+    <row r="119" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>60</v>
       </c>
@@ -1970,7 +1965,7 @@
         <v>75</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="120">
+    <row r="120" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>60</v>
       </c>
@@ -1981,7 +1976,7 @@
         <v>77</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="121">
+    <row r="121" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>60</v>
       </c>
@@ -1992,7 +1987,7 @@
         <v>86</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="122">
+    <row r="122" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>60</v>
       </c>
@@ -2003,7 +1998,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="123">
+    <row r="123" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
         <v>60</v>
       </c>
@@ -2014,7 +2009,7 @@
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="124">
+    <row r="124" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>60</v>
       </c>
@@ -2025,7 +2020,7 @@
         <v>87</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="125">
+    <row r="125" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>60</v>
       </c>
@@ -2036,7 +2031,7 @@
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="126">
+    <row r="126" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>60</v>
       </c>
@@ -2047,7 +2042,7 @@
         <v>57</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="127">
+    <row r="127" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
         <v>60</v>
       </c>
@@ -2058,7 +2053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="128">
+    <row r="128" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>60</v>
       </c>
@@ -2069,7 +2064,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="129">
+    <row r="129" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>60</v>
       </c>
@@ -2080,7 +2075,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="130">
+    <row r="130" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>60</v>
       </c>
@@ -2091,7 +2086,7 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="131">
+    <row r="131" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>60</v>
       </c>
@@ -2102,7 +2097,7 @@
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="132">
+    <row r="132" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>60</v>
       </c>
@@ -2113,7 +2108,7 @@
         <v>9.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="133">
+    <row r="133" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>60</v>
       </c>
@@ -2124,7 +2119,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="134">
+    <row r="134" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>60</v>
       </c>
@@ -2135,7 +2130,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="135">
+    <row r="135" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>60</v>
       </c>
@@ -2146,7 +2141,7 @@
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="136">
+    <row r="136" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>60</v>
       </c>
@@ -2157,7 +2152,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="137">
+    <row r="137" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
         <v>60</v>
       </c>
@@ -2168,7 +2163,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="138">
+    <row r="138" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
         <v>60</v>
       </c>
@@ -2179,7 +2174,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="139">
+    <row r="139" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
         <v>60</v>
       </c>
@@ -2190,7 +2185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="140">
+    <row r="140" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
         <v>60</v>
       </c>
@@ -2201,7 +2196,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="141">
+    <row r="141" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>60</v>
       </c>
@@ -2212,7 +2207,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="142">
+    <row r="142" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
         <v>60</v>
       </c>
@@ -2223,7 +2218,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="143">
+    <row r="143" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
         <v>60</v>
       </c>
@@ -2234,7 +2229,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="144">
+    <row r="144" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
         <v>60</v>
       </c>
@@ -2245,7 +2240,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="145">
+    <row r="145" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
         <v>60</v>
       </c>
@@ -2256,7 +2251,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="146">
+    <row r="146" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
         <v>60</v>
       </c>
@@ -2267,7 +2262,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="147">
+    <row r="147" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>60</v>
       </c>
@@ -2278,7 +2273,7 @@
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="148">
+    <row r="148" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
         <v>60</v>
       </c>
@@ -2289,7 +2284,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="149">
+    <row r="149" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
         <v>60</v>
       </c>
@@ -2300,7 +2295,7 @@
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="150">
+    <row r="150" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
         <v>60</v>
       </c>
@@ -2311,7 +2306,7 @@
         <v>99</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="151">
+    <row r="151" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
         <v>60</v>
       </c>
@@ -2322,7 +2317,7 @@
         <v>87</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="152">
+    <row r="152" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
         <v>60</v>
       </c>
@@ -2333,7 +2328,7 @@
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="153">
+    <row r="153" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
         <v>60</v>
       </c>
@@ -2344,7 +2339,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="154">
+    <row r="154" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
         <v>60</v>
       </c>
@@ -2355,7 +2350,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="155">
+    <row r="155" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
         <v>60</v>
       </c>
@@ -2366,7 +2361,7 @@
         <v>31</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="156">
+    <row r="156" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
         <v>60</v>
       </c>
@@ -2377,7 +2372,7 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="157">
+    <row r="157" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
         <v>60</v>
       </c>
@@ -2388,7 +2383,7 @@
         <v>65</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="158">
+    <row r="158" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>60</v>
       </c>
@@ -2399,7 +2394,7 @@
         <v>53</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="159">
+    <row r="159" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
         <v>60</v>
       </c>
@@ -2410,7 +2405,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="160">
+    <row r="160" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
         <v>60</v>
       </c>
@@ -2421,7 +2416,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="161">
+    <row r="161" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
         <v>60</v>
       </c>
@@ -2432,7 +2427,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="162">
+    <row r="162" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
         <v>60</v>
       </c>
@@ -2443,7 +2438,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="163">
+    <row r="163" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
         <v>60</v>
       </c>
@@ -2454,7 +2449,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="164">
+    <row r="164" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
         <v>60</v>
       </c>
@@ -2465,7 +2460,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="165">
+    <row r="165" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
         <v>60</v>
       </c>
@@ -2476,7 +2471,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="166">
+    <row r="166" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
         <v>60</v>
       </c>
@@ -2487,7 +2482,7 @@
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="167">
+    <row r="167" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
         <v>60</v>
       </c>
@@ -2498,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="168">
+    <row r="168" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
         <v>60</v>
       </c>
@@ -2509,7 +2504,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="169">
+    <row r="169" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
         <v>60</v>
       </c>
@@ -2520,7 +2515,7 @@
         <v>48</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="170">
+    <row r="170" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
         <v>60</v>
       </c>
@@ -2531,7 +2526,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="171">
+    <row r="171" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
         <v>60</v>
       </c>
@@ -2542,7 +2537,7 @@
         <v>77</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="172">
+    <row r="172" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
         <v>60</v>
       </c>
@@ -2553,7 +2548,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="173">
+    <row r="173" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
         <v>60</v>
       </c>
@@ -2564,7 +2559,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="174">
+    <row r="174" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
         <v>60</v>
       </c>
@@ -2575,7 +2570,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="175">
+    <row r="175" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
         <v>60</v>
       </c>
@@ -2586,7 +2581,7 @@
         <v>67</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="176">
+    <row r="176" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
         <v>60</v>
       </c>
@@ -2597,7 +2592,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="177">
+    <row r="177" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
         <v>60</v>
       </c>
@@ -2608,7 +2603,7 @@
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="178">
+    <row r="178" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
         <v>60</v>
       </c>
@@ -2619,7 +2614,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="179">
+    <row r="179" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
         <v>60</v>
       </c>
@@ -2630,7 +2625,7 @@
         <v>4.4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="180">
+    <row r="180" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
         <v>60</v>
       </c>
@@ -2641,7 +2636,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="181">
+    <row r="181" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
         <v>60</v>
       </c>
@@ -2652,7 +2647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="182">
+    <row r="182" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
         <v>60</v>
       </c>
@@ -2663,7 +2658,7 @@
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="183">
+    <row r="183" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
         <v>60</v>
       </c>
@@ -2674,7 +2669,7 @@
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="184">
+    <row r="184" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
         <v>60</v>
       </c>
@@ -2685,7 +2680,7 @@
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="185">
+    <row r="185" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
         <v>60</v>
       </c>
@@ -2696,7 +2691,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="186">
+    <row r="186" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
         <v>60</v>
       </c>
@@ -2707,7 +2702,7 @@
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="187">
+    <row r="187" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
         <v>60</v>
       </c>
@@ -2718,7 +2713,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="188">
+    <row r="188" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
         <v>60</v>
       </c>
@@ -2729,7 +2724,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="189">
+    <row r="189" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
         <v>60</v>
       </c>
@@ -2740,7 +2735,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="190">
+    <row r="190" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
         <v>60</v>
       </c>
@@ -2751,7 +2746,7 @@
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="191">
+    <row r="191" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
         <v>60</v>
       </c>
@@ -2762,7 +2757,7 @@
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="192">
+    <row r="192" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
         <v>60</v>
       </c>
@@ -2773,7 +2768,7 @@
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="193">
+    <row r="193" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
         <v>60</v>
       </c>
@@ -2784,7 +2779,7 @@
         <v>95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="194">
+    <row r="194" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
         <v>60</v>
       </c>
@@ -2795,7 +2790,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="195">
+    <row r="195" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
         <v>60</v>
       </c>
@@ -2806,7 +2801,7 @@
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="196">
+    <row r="196" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
         <v>60</v>
       </c>
@@ -2817,7 +2812,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="197">
+    <row r="197" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
         <v>60</v>
       </c>
@@ -2828,7 +2823,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="198">
+    <row r="198" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
         <v>60</v>
       </c>
@@ -2839,7 +2834,7 @@
         <v>58</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="199">
+    <row r="199" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
         <v>60</v>
       </c>
@@ -2850,7 +2845,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="200">
+    <row r="200" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
         <v>60</v>
       </c>
@@ -2861,7 +2856,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="201">
+    <row r="201" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
         <v>60</v>
       </c>
@@ -2872,7 +2867,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="202">
+    <row r="202" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
         <v>60</v>
       </c>
@@ -2883,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="203">
+    <row r="203" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
         <v>60</v>
       </c>
@@ -2894,7 +2889,7 @@
         <v>59</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="204">
+    <row r="204" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
         <v>60</v>
       </c>
@@ -2905,7 +2900,7 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="205">
+    <row r="205" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
         <v>60</v>
       </c>
@@ -2916,7 +2911,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="206">
+    <row r="206" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
         <v>60</v>
       </c>
@@ -2927,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="207">
+    <row r="207" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
         <v>60</v>
       </c>
@@ -2938,7 +2933,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="208">
+    <row r="208" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
         <v>60</v>
       </c>
@@ -2949,7 +2944,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="209">
+    <row r="209" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
         <v>60</v>
       </c>
@@ -2960,7 +2955,7 @@
         <v>1.1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="210">
+    <row r="210" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
         <v>60</v>
       </c>
@@ -2971,7 +2966,7 @@
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="211">
+    <row r="211" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
         <v>60</v>
       </c>
@@ -2982,7 +2977,7 @@
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="212">
+    <row r="212" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
         <v>60</v>
       </c>
@@ -2993,7 +2988,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="213">
+    <row r="213" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
         <v>60</v>
       </c>
@@ -3004,7 +2999,7 @@
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="214">
+    <row r="214" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
         <v>60</v>
       </c>
@@ -3015,7 +3010,7 @@
         <v>57</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="215">
+    <row r="215" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
         <v>60</v>
       </c>
@@ -3026,7 +3021,7 @@
         <v>76</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="216">
+    <row r="216" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
         <v>60</v>
       </c>
@@ -3037,7 +3032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="217">
+    <row r="217" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
         <v>60</v>
       </c>
@@ -3048,7 +3043,7 @@
         <v>77</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="218">
+    <row r="218" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
         <v>60</v>
       </c>
@@ -3059,7 +3054,7 @@
         <v>89</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="219">
+    <row r="219" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
         <v>60</v>
       </c>
@@ -3070,7 +3065,7 @@
         <v>88</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="220">
+    <row r="220" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
         <v>60</v>
       </c>
@@ -3081,7 +3076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="221">
+    <row r="221" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
         <v>60</v>
       </c>
@@ -3092,7 +3087,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="222">
+    <row r="222" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
         <v>60</v>
       </c>
@@ -3103,7 +3098,7 @@
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="223">
+    <row r="223" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
         <v>60</v>
       </c>
@@ -3114,7 +3109,7 @@
         <v>64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="224">
+    <row r="224" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
         <v>60</v>
       </c>
@@ -3125,7 +3120,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="225">
+    <row r="225" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
         <v>60</v>
       </c>
@@ -3136,7 +3131,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="226">
+    <row r="226" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
         <v>60</v>
       </c>
@@ -3147,7 +3142,7 @@
         <v>86</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="227">
+    <row r="227" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
         <v>60</v>
       </c>
@@ -3158,7 +3153,7 @@
         <v>98</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="228">
+    <row r="228" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
         <v>60</v>
       </c>
@@ -3169,7 +3164,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="229">
+    <row r="229" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
         <v>60</v>
       </c>
@@ -3180,7 +3175,7 @@
         <v>54</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="230">
+    <row r="230" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
         <v>60</v>
       </c>
@@ -3191,7 +3186,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="231">
+    <row r="231" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
         <v>60</v>
       </c>
@@ -3202,7 +3197,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="232">
+    <row r="232" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
         <v>60</v>
       </c>
@@ -3213,7 +3208,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="233">
+    <row r="233" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
         <v>60</v>
       </c>
@@ -3224,7 +3219,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="234">
+    <row r="234" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
         <v>60</v>
       </c>
@@ -3235,7 +3230,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="235">
+    <row r="235" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
         <v>60</v>
       </c>
@@ -3246,7 +3241,7 @@
         <v>98</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="236">
+    <row r="236" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
         <v>60</v>
       </c>
@@ -3257,7 +3252,7 @@
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="237">
+    <row r="237" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
         <v>60</v>
       </c>
@@ -3268,7 +3263,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="238">
+    <row r="238" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
         <v>60</v>
       </c>
@@ -3279,7 +3274,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="239">
+    <row r="239" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
         <v>60</v>
       </c>
@@ -3290,7 +3285,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="240">
+    <row r="240" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
         <v>60</v>
       </c>
@@ -3301,7 +3296,7 @@
         <v>86</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="241">
+    <row r="241" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
         <v>60</v>
       </c>
@@ -3312,7 +3307,7 @@
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="242">
+    <row r="242" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
         <v>60</v>
       </c>
@@ -3323,7 +3318,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="243">
+    <row r="243" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
         <v>60</v>
       </c>
@@ -3334,7 +3329,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="244">
+    <row r="244" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
         <v>60</v>
       </c>
@@ -3345,7 +3340,7 @@
         <v>76</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="245">
+    <row r="245" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
         <v>60</v>
       </c>
@@ -3356,7 +3351,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="246">
+    <row r="246" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
         <v>60</v>
       </c>
@@ -3367,7 +3362,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="247">
+    <row r="247" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
         <v>60</v>
       </c>
@@ -3378,7 +3373,7 @@
         <v>69</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="248">
+    <row r="248" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
         <v>60</v>
       </c>
@@ -3389,7 +3384,7 @@
         <v>83</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="249">
+    <row r="249" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
         <v>60</v>
       </c>
@@ -3400,7 +3395,7 @@
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="250">
+    <row r="250" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
         <v>60</v>
       </c>
@@ -3411,7 +3406,7 @@
         <v>46</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="251">
+    <row r="251" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
         <v>60</v>
       </c>
@@ -3422,7 +3417,7 @@
         <v>88</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="252">
+    <row r="252" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
         <v>60</v>
       </c>
@@ -3433,7 +3428,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="253">
+    <row r="253" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
         <v>60</v>
       </c>
@@ -3444,7 +3439,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="254">
+    <row r="254" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
         <v>60</v>
       </c>
@@ -3455,7 +3450,7 @@
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="255">
+    <row r="255" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
         <v>60</v>
       </c>
@@ -3466,7 +3461,7 @@
         <v>88</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="256">
+    <row r="256" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
         <v>60</v>
       </c>
@@ -3477,7 +3472,7 @@
         <v>73</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="257">
+    <row r="257" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
         <v>60</v>
       </c>
@@ -3488,7 +3483,7 @@
         <v>99</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="258">
+    <row r="258" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
         <v>60</v>
       </c>
@@ -3499,7 +3494,7 @@
         <v>95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="259">
+    <row r="259" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
         <v>60</v>
       </c>
@@ -3510,7 +3505,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="260">
+    <row r="260" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
         <v>60</v>
       </c>
@@ -3521,7 +3516,7 @@
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="261">
+    <row r="261" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
         <v>60</v>
       </c>
@@ -3532,7 +3527,7 @@
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="262">
+    <row r="262" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
         <v>60</v>
       </c>
@@ -3543,7 +3538,7 @@
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="263">
+    <row r="263" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
         <v>60</v>
       </c>
@@ -3554,7 +3549,7 @@
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="264">
+    <row r="264" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
         <v>60</v>
       </c>
@@ -3565,7 +3560,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="265">
+    <row r="265" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
         <v>60</v>
       </c>
@@ -3576,7 +3571,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="266">
+    <row r="266" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
         <v>60</v>
       </c>
@@ -3587,7 +3582,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="267">
+    <row r="267" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
         <v>60</v>
       </c>
@@ -3598,7 +3593,7 @@
         <v>83</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="268">
+    <row r="268" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
         <v>60</v>
       </c>
@@ -3609,7 +3604,7 @@
         <v>43</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="269">
+    <row r="269" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
         <v>60</v>
       </c>
@@ -3620,7 +3615,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="270">
+    <row r="270" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
         <v>60</v>
       </c>
@@ -3631,7 +3626,7 @@
         <v>67</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="271">
+    <row r="271" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
         <v>60</v>
       </c>
@@ -3642,7 +3637,7 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="272">
+    <row r="272" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
         <v>60</v>
       </c>
@@ -3653,7 +3648,7 @@
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="273">
+    <row r="273" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
         <v>60</v>
       </c>
@@ -3664,7 +3659,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="274">
+    <row r="274" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
         <v>60</v>
       </c>
@@ -3675,7 +3670,7 @@
         <v>88</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="275">
+    <row r="275" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
         <v>60</v>
       </c>
@@ -3686,7 +3681,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="276">
+    <row r="276" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
         <v>60</v>
       </c>
@@ -3697,7 +3692,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="277">
+    <row r="277" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
         <v>60</v>
       </c>
@@ -3708,7 +3703,7 @@
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="278">
+    <row r="278" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
         <v>60</v>
       </c>
@@ -3719,7 +3714,7 @@
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="279">
+    <row r="279" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
         <v>60</v>
       </c>
@@ -3730,7 +3725,7 @@
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="280">
+    <row r="280" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
         <v>60</v>
       </c>
@@ -3741,7 +3736,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="281">
+    <row r="281" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
         <v>60</v>
       </c>
@@ -3752,7 +3747,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="282">
+    <row r="282" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
         <v>60</v>
       </c>
@@ -3763,7 +3758,7 @@
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="283">
+    <row r="283" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
         <v>60</v>
       </c>
@@ -3774,7 +3769,7 @@
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="284">
+    <row r="284" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
         <v>60</v>
       </c>
@@ -3785,7 +3780,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="285">
+    <row r="285" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
         <v>60</v>
       </c>
@@ -3796,7 +3791,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="286">
+    <row r="286" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
         <v>60</v>
       </c>
@@ -3807,7 +3802,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="287">
+    <row r="287" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
         <v>60</v>
       </c>
@@ -3818,7 +3813,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="288">
+    <row r="288" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
         <v>60</v>
       </c>
@@ -3829,7 +3824,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="289">
+    <row r="289" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
         <v>60</v>
       </c>
@@ -3840,7 +3835,7 @@
         <v>51</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="290">
+    <row r="290" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
         <v>60</v>
       </c>
@@ -3851,7 +3846,7 @@
         <v>62</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="291">
+    <row r="291" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
         <v>60</v>
       </c>
@@ -3862,7 +3857,7 @@
         <v>73</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="292">
+    <row r="292" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
         <v>60</v>
       </c>
@@ -3873,7 +3868,7 @@
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="293">
+    <row r="293" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="0" t="s">
         <v>60</v>
       </c>
@@ -3884,7 +3879,7 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="294">
+    <row r="294" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="s">
         <v>60</v>
       </c>
@@ -3895,7 +3890,7 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="295">
+    <row r="295" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="s">
         <v>60</v>
       </c>
@@ -3906,7 +3901,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="296">
+    <row r="296" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
         <v>60</v>
       </c>
@@ -3917,7 +3912,7 @@
         <v>72</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="297">
+    <row r="297" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
         <v>60</v>
       </c>
@@ -3928,7 +3923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="298">
+    <row r="298" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
         <v>60</v>
       </c>
@@ -3939,7 +3934,7 @@
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="299">
+    <row r="299" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
         <v>60</v>
       </c>
@@ -3950,7 +3945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="300">
+    <row r="300" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
         <v>60</v>
       </c>
@@ -3961,7 +3956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="301">
+    <row r="301" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
         <v>60</v>
       </c>
@@ -3972,7 +3967,7 @@
         <v>76</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="302">
+    <row r="302" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
         <v>60</v>
       </c>
@@ -3983,7 +3978,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="303">
+    <row r="303" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="s">
         <v>60</v>
       </c>
@@ -3994,7 +3989,7 @@
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="304">
+    <row r="304" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
         <v>60</v>
       </c>
@@ -4005,7 +4000,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="305">
+    <row r="305" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="s">
         <v>60</v>
       </c>
@@ -4016,7 +4011,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="306">
+    <row r="306" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
         <v>60</v>
       </c>
@@ -4027,7 +4022,7 @@
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="307">
+    <row r="307" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
         <v>60</v>
       </c>
@@ -4038,7 +4033,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="308">
+    <row r="308" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="s">
         <v>60</v>
       </c>
@@ -4049,7 +4044,7 @@
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="309">
+    <row r="309" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
         <v>60</v>
       </c>
@@ -4060,7 +4055,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="310">
+    <row r="310" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
         <v>60</v>
       </c>
@@ -4071,7 +4066,7 @@
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="311">
+    <row r="311" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
         <v>60</v>
       </c>
@@ -4082,7 +4077,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="312">
+    <row r="312" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
         <v>60</v>
       </c>
@@ -4093,7 +4088,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="313">
+    <row r="313" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="s">
         <v>60</v>
       </c>
@@ -4104,7 +4099,7 @@
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="314">
+    <row r="314" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
         <v>60</v>
       </c>
@@ -4115,7 +4110,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="315">
+    <row r="315" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="s">
         <v>60</v>
       </c>
@@ -4126,7 +4121,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="316">
+    <row r="316" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="s">
         <v>60</v>
       </c>
@@ -4137,7 +4132,7 @@
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="317">
+    <row r="317" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="s">
         <v>60</v>
       </c>
@@ -4148,7 +4143,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="318">
+    <row r="318" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="s">
         <v>60</v>
       </c>
@@ -4159,7 +4154,7 @@
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="319">
+    <row r="319" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="s">
         <v>60</v>
       </c>
@@ -4170,7 +4165,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="320">
+    <row r="320" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="s">
         <v>60</v>
       </c>
@@ -4181,7 +4176,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="321">
+    <row r="321" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="s">
         <v>60</v>
       </c>
@@ -4192,7 +4187,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="322">
+    <row r="322" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="s">
         <v>60</v>
       </c>
@@ -4203,7 +4198,7 @@
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="323">
+    <row r="323" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0" t="s">
         <v>60</v>
       </c>
@@ -4214,7 +4209,7 @@
         <v>84</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="324">
+    <row r="324" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="s">
         <v>60</v>
       </c>
@@ -4225,7 +4220,7 @@
         <v>98</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="325">
+    <row r="325" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="s">
         <v>60</v>
       </c>
@@ -4236,7 +4231,7 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="326">
+    <row r="326" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="0" t="s">
         <v>60</v>
       </c>
@@ -4247,7 +4242,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="327">
+    <row r="327" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="0" t="s">
         <v>60</v>
       </c>
@@ -4258,7 +4253,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="328">
+    <row r="328" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="0" t="s">
         <v>60</v>
       </c>
@@ -4269,7 +4264,7 @@
         <v>87</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="329">
+    <row r="329" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="0" t="s">
         <v>60</v>
       </c>
@@ -4280,7 +4275,7 @@
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="330">
+    <row r="330" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="0" t="s">
         <v>60</v>
       </c>
@@ -4291,7 +4286,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="331">
+    <row r="331" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="0" t="s">
         <v>60</v>
       </c>
@@ -4302,7 +4297,7 @@
         <v>63</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="332">
+    <row r="332" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="0" t="s">
         <v>60</v>
       </c>
@@ -4313,7 +4308,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="333">
+    <row r="333" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="0" t="s">
         <v>60</v>
       </c>
@@ -4324,7 +4319,7 @@
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="334">
+    <row r="334" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="0" t="s">
         <v>60</v>
       </c>
@@ -4335,7 +4330,7 @@
         <v>99</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="335">
+    <row r="335" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="s">
         <v>60</v>
       </c>
@@ -4346,7 +4341,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="336">
+    <row r="336" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="0" t="s">
         <v>60</v>
       </c>
@@ -4357,7 +4352,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="337">
+    <row r="337" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="0" t="s">
         <v>60</v>
       </c>
@@ -4368,7 +4363,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="338">
+    <row r="338" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="0" t="s">
         <v>60</v>
       </c>
@@ -4379,7 +4374,7 @@
         <v>71</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="339">
+    <row r="339" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="0" t="s">
         <v>60</v>
       </c>
@@ -4390,7 +4385,7 @@
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="340">
+    <row r="340" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="0" t="s">
         <v>60</v>
       </c>
@@ -4401,7 +4396,7 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="341">
+    <row r="341" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="0" t="s">
         <v>60</v>
       </c>
@@ -4412,7 +4407,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="342">
+    <row r="342" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="0" t="s">
         <v>60</v>
       </c>
@@ -4423,7 +4418,7 @@
         <v>86</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="343">
+    <row r="343" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="0" t="s">
         <v>60</v>
       </c>
@@ -4434,7 +4429,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="344">
+    <row r="344" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="0" t="s">
         <v>60</v>
       </c>
@@ -4445,7 +4440,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="345">
+    <row r="345" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="0" t="s">
         <v>60</v>
       </c>
@@ -4456,7 +4451,7 @@
         <v>84</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="346">
+    <row r="346" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="0" t="s">
         <v>60</v>
       </c>
@@ -4467,7 +4462,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="347">
+    <row r="347" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="0" t="s">
         <v>60</v>
       </c>
@@ -4478,7 +4473,7 @@
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="348">
+    <row r="348" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="0" t="s">
         <v>60</v>
       </c>
@@ -4489,7 +4484,7 @@
         <v>67</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="349">
+    <row r="349" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="0" t="s">
         <v>60</v>
       </c>
@@ -4500,7 +4495,7 @@
         <v>95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="350">
+    <row r="350" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="0" t="s">
         <v>60</v>
       </c>
@@ -4511,7 +4506,7 @@
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="351">
+    <row r="351" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="0" t="s">
         <v>60</v>
       </c>
@@ -4522,7 +4517,7 @@
         <v>73</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="352">
+    <row r="352" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="0" t="s">
         <v>60</v>
       </c>
@@ -4533,7 +4528,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="353">
+    <row r="353" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="0" t="s">
         <v>60</v>
       </c>
@@ -4544,7 +4539,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="354">
+    <row r="354" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="0" t="s">
         <v>60</v>
       </c>
@@ -4555,7 +4550,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="355">
+    <row r="355" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="0" t="s">
         <v>60</v>
       </c>
@@ -4566,7 +4561,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="356">
+    <row r="356" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="0" t="s">
         <v>60</v>
       </c>
@@ -4577,7 +4572,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="357">
+    <row r="357" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="0" t="s">
         <v>60</v>
       </c>
@@ -4588,7 +4583,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="358">
+    <row r="358" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="0" t="s">
         <v>60</v>
       </c>
@@ -4599,7 +4594,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="359">
+    <row r="359" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="0" t="s">
         <v>60</v>
       </c>
@@ -4610,7 +4605,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="360">
+    <row r="360" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="0" t="s">
         <v>60</v>
       </c>
@@ -4621,7 +4616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="361">
+    <row r="361" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="0" t="s">
         <v>60</v>
       </c>
@@ -4632,7 +4627,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="362">
+    <row r="362" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="0" t="s">
         <v>60</v>
       </c>
@@ -4643,7 +4638,7 @@
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="363">
+    <row r="363" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="0" t="s">
         <v>60</v>
       </c>
@@ -4654,7 +4649,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="364">
+    <row r="364" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="0" t="s">
         <v>60</v>
       </c>
@@ -4665,7 +4660,7 @@
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="365">
+    <row r="365" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="0" t="s">
         <v>60</v>
       </c>
@@ -4676,7 +4671,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="366">
+    <row r="366" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="0" t="s">
         <v>60</v>
       </c>
@@ -4687,7 +4682,7 @@
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="367">
+    <row r="367" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="0" t="s">
         <v>60</v>
       </c>
@@ -4698,7 +4693,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="368">
+    <row r="368" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="0" t="s">
         <v>60</v>
       </c>
@@ -4709,7 +4704,7 @@
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="369">
+    <row r="369" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="0" t="s">
         <v>60</v>
       </c>
@@ -4720,7 +4715,7 @@
         <v>88</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="370">
+    <row r="370" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="0" t="s">
         <v>60</v>
       </c>
@@ -4731,7 +4726,7 @@
         <v>83</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="371">
+    <row r="371" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="0" t="s">
         <v>60</v>
       </c>
@@ -4742,7 +4737,7 @@
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="372">
+    <row r="372" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="0" t="s">
         <v>60</v>
       </c>
@@ -4753,7 +4748,7 @@
         <v>89</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="373">
+    <row r="373" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="0" t="s">
         <v>60</v>
       </c>
@@ -4764,7 +4759,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="374">
+    <row r="374" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="0" t="s">
         <v>60</v>
       </c>
@@ -4775,7 +4770,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="375">
+    <row r="375" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="0" t="s">
         <v>60</v>
       </c>
@@ -4786,7 +4781,7 @@
         <v>82</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="376">
+    <row r="376" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="0" t="s">
         <v>60</v>
       </c>
@@ -4797,7 +4792,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="377">
+    <row r="377" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="0" t="s">
         <v>60</v>
       </c>
@@ -4808,7 +4803,7 @@
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="378">
+    <row r="378" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="0" t="s">
         <v>60</v>
       </c>
@@ -4819,7 +4814,7 @@
         <v>55</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="379">
+    <row r="379" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="0" t="s">
         <v>60</v>
       </c>
@@ -4830,7 +4825,7 @@
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="380">
+    <row r="380" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="0" t="s">
         <v>60</v>
       </c>
@@ -4841,7 +4836,7 @@
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="381">
+    <row r="381" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="0" t="s">
         <v>60</v>
       </c>
@@ -4852,7 +4847,7 @@
         <v>38</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="382">
+    <row r="382" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="0" t="s">
         <v>60</v>
       </c>
@@ -4863,7 +4858,7 @@
         <v>63</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="383">
+    <row r="383" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="0" t="s">
         <v>60</v>
       </c>
@@ -4874,7 +4869,7 @@
         <v>89</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="384">
+    <row r="384" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="0" t="s">
         <v>60</v>
       </c>
@@ -4885,7 +4880,7 @@
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="385">
+    <row r="385" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="0" t="s">
         <v>60</v>
       </c>
@@ -4896,7 +4891,7 @@
         <v>82</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="386">
+    <row r="386" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="0" t="s">
         <v>60</v>
       </c>
@@ -4907,7 +4902,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="387">
+    <row r="387" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="0" t="s">
         <v>60</v>
       </c>
@@ -4918,7 +4913,7 @@
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="388">
+    <row r="388" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="0" t="s">
         <v>60</v>
       </c>
@@ -4929,7 +4924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="389">
+    <row r="389" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="0" t="s">
         <v>60</v>
       </c>
@@ -4940,7 +4935,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="390">
+    <row r="390" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="0" t="s">
         <v>60</v>
       </c>
@@ -4951,7 +4946,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="391">
+    <row r="391" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="0" t="s">
         <v>60</v>
       </c>
@@ -4962,7 +4957,7 @@
         <v>48</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="392">
+    <row r="392" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="0" t="s">
         <v>60</v>
       </c>
@@ -4973,7 +4968,7 @@
         <v>72</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="393">
+    <row r="393" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="0" t="s">
         <v>60</v>
       </c>
@@ -4984,7 +4979,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="394">
+    <row r="394" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="0" t="s">
         <v>60</v>
       </c>
@@ -4995,7 +4990,7 @@
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="395">
+    <row r="395" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="0" t="s">
         <v>60</v>
       </c>
@@ -5006,7 +5001,7 @@
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="396">
+    <row r="396" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="0" t="s">
         <v>60</v>
       </c>
@@ -5017,7 +5012,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="397">
+    <row r="397" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="0" t="s">
         <v>60</v>
       </c>
@@ -5028,7 +5023,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="398">
+    <row r="398" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="0" t="s">
         <v>60</v>
       </c>
@@ -5039,7 +5034,7 @@
         <v>34</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="399">
+    <row r="399" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="0" t="s">
         <v>60</v>
       </c>
@@ -5050,7 +5045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="400">
+    <row r="400" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="0" t="s">
         <v>60</v>
       </c>
@@ -5061,7 +5056,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="401">
+    <row r="401" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="s">
         <v>60</v>
       </c>
@@ -5072,7 +5067,7 @@
         <v>88</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="402">
+    <row r="402" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="0" t="s">
         <v>60</v>
       </c>
@@ -5083,7 +5078,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="403">
+    <row r="403" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="0" t="s">
         <v>60</v>
       </c>
@@ -5094,7 +5089,7 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="404">
+    <row r="404" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="0" t="s">
         <v>60</v>
       </c>
@@ -5105,7 +5100,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="405">
+    <row r="405" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="0" t="s">
         <v>60</v>
       </c>
@@ -5116,7 +5111,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="406">
+    <row r="406" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="0" t="s">
         <v>60</v>
       </c>
@@ -5127,7 +5122,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="407">
+    <row r="407" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="0" t="s">
         <v>60</v>
       </c>
@@ -5138,7 +5133,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="408">
+    <row r="408" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="0" t="s">
         <v>60</v>
       </c>
@@ -5149,7 +5144,7 @@
         <v>62</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="409">
+    <row r="409" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="0" t="s">
         <v>60</v>
       </c>
@@ -5160,7 +5155,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="410">
+    <row r="410" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="0" t="s">
         <v>60</v>
       </c>
@@ -5171,7 +5166,7 @@
         <v>35</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="411">
+    <row r="411" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="0" t="s">
         <v>60</v>
       </c>
@@ -5182,7 +5177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="412">
+    <row r="412" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="0" t="s">
         <v>60</v>
       </c>
@@ -5193,7 +5188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="413">
+    <row r="413" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="0" t="s">
         <v>60</v>
       </c>
@@ -5204,7 +5199,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="414">
+    <row r="414" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="0" t="s">
         <v>60</v>
       </c>
@@ -5215,7 +5210,7 @@
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="415">
+    <row r="415" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="0" t="s">
         <v>60</v>
       </c>
@@ -5226,7 +5221,7 @@
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="416">
+    <row r="416" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="0" t="s">
         <v>60</v>
       </c>
@@ -5237,7 +5232,7 @@
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="417">
+    <row r="417" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="0" t="s">
         <v>60</v>
       </c>
@@ -5248,7 +5243,7 @@
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="418">
+    <row r="418" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="0" t="s">
         <v>60</v>
       </c>
@@ -5259,7 +5254,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="419">
+    <row r="419" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="0" t="s">
         <v>60</v>
       </c>
@@ -5270,7 +5265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="420">
+    <row r="420" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="0" t="s">
         <v>60</v>
       </c>
@@ -5281,7 +5276,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="421">
+    <row r="421" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="0" t="s">
         <v>60</v>
       </c>
@@ -5292,7 +5287,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="422">
+    <row r="422" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="0" t="s">
         <v>60</v>
       </c>
@@ -5303,7 +5298,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="423">
+    <row r="423" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="0" t="s">
         <v>60</v>
       </c>
@@ -5314,7 +5309,7 @@
         <v>78</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="424">
+    <row r="424" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="0" t="s">
         <v>60</v>
       </c>
@@ -5325,7 +5320,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="425">
+    <row r="425" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="0" t="s">
         <v>60</v>
       </c>
@@ -5336,7 +5331,7 @@
         <v>77</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="426">
+    <row r="426" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="0" t="s">
         <v>60</v>
       </c>
@@ -5347,7 +5342,7 @@
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="427">
+    <row r="427" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="s">
         <v>60</v>
       </c>
@@ -5358,7 +5353,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="428">
+    <row r="428" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="s">
         <v>60</v>
       </c>
@@ -5369,7 +5364,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="429">
+    <row r="429" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="0" t="s">
         <v>60</v>
       </c>
@@ -5380,7 +5375,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="430">
+    <row r="430" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="0" t="s">
         <v>60</v>
       </c>
@@ -5391,7 +5386,7 @@
         <v>89</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="431">
+    <row r="431" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="0" t="s">
         <v>60</v>
       </c>
@@ -5402,7 +5397,7 @@
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="432">
+    <row r="432" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="0" t="s">
         <v>60</v>
       </c>
@@ -5413,7 +5408,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="433">
+    <row r="433" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="0" t="s">
         <v>60</v>
       </c>
@@ -5424,7 +5419,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="434">
+    <row r="434" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="0" t="s">
         <v>60</v>
       </c>
@@ -5435,7 +5430,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="435">
+    <row r="435" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="0" t="s">
         <v>60</v>
       </c>
@@ -5446,7 +5441,7 @@
         <v>87</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="436">
+    <row r="436" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="0" t="s">
         <v>60</v>
       </c>
@@ -5457,7 +5452,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="437">
+    <row r="437" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="0" t="s">
         <v>60</v>
       </c>
@@ -5468,7 +5463,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="438">
+    <row r="438" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="0" t="s">
         <v>60</v>
       </c>
@@ -5479,7 +5474,7 @@
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="439">
+    <row r="439" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="0" t="s">
         <v>60</v>
       </c>
@@ -5490,7 +5485,7 @@
         <v>69</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="440">
+    <row r="440" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="0" t="s">
         <v>60</v>
       </c>
@@ -5501,7 +5496,7 @@
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="441">
+    <row r="441" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="0" t="s">
         <v>60</v>
       </c>
@@ -5512,7 +5507,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="442">
+    <row r="442" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="0" t="s">
         <v>60</v>
       </c>
@@ -5523,7 +5518,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="443">
+    <row r="443" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="0" t="s">
         <v>60</v>
       </c>
@@ -5537,7 +5532,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>